<commit_message>
update spreadsheets and gemfile with new version
</commit_message>
<xml_diff>
--- a/projects/SimpleContinuousExample.xlsx
+++ b/projects/SimpleContinuousExample.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23256" windowHeight="13176" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="9" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Outputs!$A$2:$I$15</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Variables!$A$2:$Y$15</definedName>
   </definedNames>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1875" uniqueCount="527">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1873" uniqueCount="524">
   <si>
     <t>type</t>
   </si>
@@ -1585,15 +1585,6 @@
   </si>
   <si>
     <t>normal_uncertain</t>
-  </si>
-  <si>
-    <t>[10,30,50,80]</t>
-  </si>
-  <si>
-    <t>[0.05,0.1,0.45,0.4]</t>
-  </si>
-  <si>
-    <t>discrete_uncertain</t>
   </si>
   <si>
     <t>Ruby Continuous Variables Example Problem</t>
@@ -1668,7 +1659,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1723,12 +1714,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1739,7 +1724,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1311">
+  <cellStyleXfs count="1315">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3051,8 +3036,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -3122,25 +3111,15 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1311">
+  <cellStyles count="1315">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -3796,6 +3775,8 @@
     <cellStyle name="Followed Hyperlink" xfId="1306" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1308" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1310" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1312" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1314" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -4451,6 +4432,8 @@
     <cellStyle name="Hyperlink" xfId="1305" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1307" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1309" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1311" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1313" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -4756,17 +4739,17 @@
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="50.77734375" customWidth="1"/>
+    <col min="1" max="1" width="50.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:1">
       <c r="A12" t="s">
         <v>49</v>
       </c>
@@ -4786,21 +4769,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="25.77734375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="26.77734375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="32.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.83203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="26.83203125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="32.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="47" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="10.77734375" style="1"/>
+    <col min="6" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5">
       <c r="A1" s="22"/>
       <c r="B1" s="27"/>
       <c r="C1" s="22"/>
@@ -4809,7 +4792,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" s="13" customFormat="1">
       <c r="A2" s="12" t="s">
         <v>446</v>
       </c>
@@ -4818,7 +4801,7 @@
       <c r="D2" s="14"/>
       <c r="E2" s="14"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5">
       <c r="A3" s="1" t="s">
         <v>447</v>
       </c>
@@ -4829,7 +4812,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="28">
       <c r="A4" s="1" t="s">
         <v>480</v>
       </c>
@@ -4840,7 +4823,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="28">
       <c r="A5" s="1" t="s">
         <v>504</v>
       </c>
@@ -4851,7 +4834,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="56">
       <c r="A6" s="1" t="s">
         <v>506</v>
       </c>
@@ -4862,7 +4845,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5">
       <c r="A7" s="1" t="s">
         <v>460</v>
       </c>
@@ -4881,7 +4864,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="28">
       <c r="A8" s="1" t="s">
         <v>461</v>
       </c>
@@ -4900,7 +4883,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5">
       <c r="A9" s="1" t="s">
         <v>483</v>
       </c>
@@ -4913,7 +4896,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="11" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" s="13" customFormat="1">
       <c r="A11" s="12" t="s">
         <v>33</v>
       </c>
@@ -4922,18 +4905,18 @@
       <c r="D11" s="14"/>
       <c r="E11" s="14"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5">
       <c r="A12" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B12" s="25" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>508</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5">
       <c r="A13" s="1" t="s">
         <v>30</v>
       </c>
@@ -4944,7 +4927,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5">
       <c r="A14" s="1" t="s">
         <v>31</v>
       </c>
@@ -4952,7 +4935,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5">
       <c r="A15" s="1" t="s">
         <v>492</v>
       </c>
@@ -4963,7 +4946,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5">
       <c r="A16" s="1" t="s">
         <v>493</v>
       </c>
@@ -4974,7 +4957,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5">
       <c r="A17" s="1" t="s">
         <v>494</v>
       </c>
@@ -4985,7 +4968,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5">
       <c r="A18" s="1" t="s">
         <v>496</v>
       </c>
@@ -4996,10 +4979,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B19" s="25"/>
-    </row>
-    <row r="20" spans="1:5" s="2" customFormat="1" ht="72" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" s="2" customFormat="1" ht="56">
       <c r="A20" s="12" t="s">
         <v>32</v>
       </c>
@@ -5010,7 +4990,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5">
       <c r="A21" s="1" t="s">
         <v>475</v>
       </c>
@@ -5018,7 +4998,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:5" s="2" customFormat="1" ht="72" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" s="2" customFormat="1" ht="56">
       <c r="A23" s="12" t="s">
         <v>471</v>
       </c>
@@ -5029,7 +5009,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5">
       <c r="A24" s="1" t="s">
         <v>24</v>
       </c>
@@ -5037,7 +5017,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5">
       <c r="A25" s="1" t="s">
         <v>4</v>
       </c>
@@ -5045,7 +5025,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="27" spans="1:5" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" s="2" customFormat="1" ht="28">
       <c r="A27" s="12" t="s">
         <v>38</v>
       </c>
@@ -5058,7 +5038,7 @@
       <c r="D27" s="12"/>
       <c r="E27" s="14"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5">
       <c r="A28" s="1" t="s">
         <v>34</v>
       </c>
@@ -5066,7 +5046,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="30" spans="1:5" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" s="2" customFormat="1" ht="28">
       <c r="A30" s="12" t="s">
         <v>35</v>
       </c>
@@ -5083,24 +5063,24 @@
         <v>468</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" ht="28">
       <c r="A31" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B31" s="25" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>48</v>
       </c>
       <c r="D31" s="24" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>469</v>
       </c>
     </row>
-    <row r="33" spans="1:5" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" s="2" customFormat="1" ht="42">
       <c r="A33" s="12" t="s">
         <v>40</v>
       </c>
@@ -5144,30 +5124,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="120" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A23" sqref="A23"/>
+      <selection pane="bottomLeft" activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="15.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="36.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="54.77734375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="54.83203125" style="1" customWidth="1"/>
     <col min="4" max="4" width="42.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.5" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.6640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.44140625" style="1"/>
+    <col min="7" max="7" width="11.5" style="1"/>
     <col min="8" max="8" width="14" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.44140625" style="5"/>
-    <col min="10" max="17" width="11.44140625" style="1"/>
-    <col min="18" max="18" width="46.109375" style="1" customWidth="1"/>
-    <col min="19" max="21" width="11.44140625" style="1"/>
+    <col min="9" max="9" width="11.5" style="5"/>
+    <col min="10" max="17" width="11.5" style="1"/>
+    <col min="18" max="18" width="46.1640625" style="1" customWidth="1"/>
+    <col min="19" max="21" width="11.5" style="1"/>
     <col min="22" max="22" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="16384" width="11.44140625" style="1"/>
+    <col min="23" max="16384" width="11.5" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:24" ht="18">
       <c r="A1" s="6"/>
       <c r="B1" s="6"/>
       <c r="C1" s="8" t="s">
@@ -5192,16 +5172,16 @@
       <c r="P1" s="6"/>
       <c r="Q1" s="6"/>
       <c r="R1" s="6"/>
-      <c r="S1" s="39" t="s">
+      <c r="S1" s="35" t="s">
         <v>69</v>
       </c>
-      <c r="T1" s="39"/>
-      <c r="U1" s="39"/>
-      <c r="V1" s="39"/>
-      <c r="W1" s="39"/>
-      <c r="X1" s="39"/>
-    </row>
-    <row r="2" spans="1:24" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="T1" s="35"/>
+      <c r="U1" s="35"/>
+      <c r="V1" s="35"/>
+      <c r="W1" s="35"/>
+      <c r="X1" s="35"/>
+    </row>
+    <row r="2" spans="1:24" s="9" customFormat="1" ht="15">
       <c r="A2" s="9" t="s">
         <v>3</v>
       </c>
@@ -5214,7 +5194,7 @@
       <c r="H2" s="10"/>
       <c r="I2" s="10"/>
     </row>
-    <row r="3" spans="1:24" s="16" customFormat="1" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24" s="16" customFormat="1" ht="45">
       <c r="A3" s="16" t="s">
         <v>1</v>
       </c>
@@ -5285,7 +5265,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:24">
       <c r="A4" s="1" t="b">
         <v>0</v>
       </c>
@@ -5296,7 +5276,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:24">
       <c r="B5" s="1" t="s">
         <v>25</v>
       </c>
@@ -5320,384 +5300,375 @@
       <c r="Q5" s="4"/>
       <c r="R5" s="2"/>
     </row>
-    <row r="6" spans="1:24" s="33" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="33" t="b">
+    <row r="6" spans="1:24">
+      <c r="A6" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="B6" s="33" t="s">
+      <c r="B6" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C6" s="33" t="s">
+      <c r="C6" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D6" s="33" t="s">
+      <c r="D6" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="I6" s="34"/>
-      <c r="J6" s="35"/>
-      <c r="K6" s="35"/>
-      <c r="L6" s="35"/>
-      <c r="M6" s="35"/>
-      <c r="N6" s="35"/>
-      <c r="O6" s="35"/>
-      <c r="Q6" s="36"/>
-      <c r="R6" s="37"/>
-    </row>
-    <row r="7" spans="1:24" s="33" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="33" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" s="33" t="s">
+      <c r="H6" s="1"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="Q6" s="4"/>
+      <c r="R6" s="2"/>
+    </row>
+    <row r="7" spans="1:24">
+      <c r="B7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D7" s="33" t="s">
+      <c r="D7" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="E7" s="33" t="s">
-        <v>2</v>
-      </c>
-      <c r="F7" s="33" t="s">
+      <c r="E7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="H7" s="33" t="s">
+      <c r="H7" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="I7" s="33" t="s">
+      <c r="I7" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="J7" s="35"/>
-      <c r="K7" s="35"/>
-      <c r="L7" s="35"/>
-      <c r="M7" s="35"/>
-      <c r="N7" s="35"/>
-      <c r="O7" s="35"/>
-      <c r="Q7" s="36"/>
-      <c r="R7" s="37"/>
-    </row>
-    <row r="8" spans="1:24" s="33" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="33" t="s">
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+      <c r="Q7" s="4"/>
+      <c r="R7" s="2"/>
+    </row>
+    <row r="8" spans="1:24">
+      <c r="B8" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="33" t="s">
+      <c r="C8" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="D8" s="33" t="s">
+      <c r="D8" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E8" s="33" t="s">
+      <c r="E8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F8" s="33" t="s">
+      <c r="F8" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="H8" s="33">
+      <c r="H8" s="1">
         <v>30</v>
       </c>
-      <c r="I8" s="34"/>
-      <c r="J8" s="35">
-        <v>0</v>
-      </c>
-      <c r="K8" s="35">
+      <c r="J8" s="3">
+        <v>0</v>
+      </c>
+      <c r="K8" s="3">
         <v>70</v>
       </c>
-      <c r="L8" s="35">
+      <c r="L8" s="3">
         <v>20</v>
       </c>
-      <c r="M8" s="35">
+      <c r="M8" s="3">
         <f>(K8-J8)/6</f>
         <v>11.666666666666666</v>
       </c>
-      <c r="N8" s="35"/>
-      <c r="O8" s="35"/>
-      <c r="P8" s="33" t="s">
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
+      <c r="P8" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="Q8" s="36"/>
-      <c r="R8" s="37"/>
-    </row>
-    <row r="9" spans="1:24" s="33" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="33" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" s="38" t="s">
+      <c r="Q8" s="4"/>
+      <c r="R8" s="2"/>
+    </row>
+    <row r="9" spans="1:24">
+      <c r="B9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="33" t="s">
         <v>55</v>
       </c>
-      <c r="D9" s="33" t="s">
+      <c r="D9" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E9" s="33" t="s">
-        <v>2</v>
-      </c>
-      <c r="F9" s="33" t="s">
+      <c r="E9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="H9" s="33">
+      <c r="H9" s="1">
         <v>150</v>
       </c>
-      <c r="I9" s="34"/>
-      <c r="J9" s="35"/>
-      <c r="K9" s="35"/>
-      <c r="L9" s="35"/>
-      <c r="M9" s="35"/>
-      <c r="N9" s="35"/>
-      <c r="O9" s="35"/>
-      <c r="Q9" s="36"/>
-      <c r="R9" s="37"/>
-    </row>
-    <row r="10" spans="1:24" s="33" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="33" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" s="33" t="s">
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
+      <c r="Q9" s="4"/>
+      <c r="R9" s="2"/>
+    </row>
+    <row r="10" spans="1:24">
+      <c r="B10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D10" s="33" t="s">
+      <c r="D10" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="E10" s="33" t="s">
-        <v>2</v>
-      </c>
-      <c r="F10" s="33" t="s">
+      <c r="E10" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="H10" s="33">
-        <v>0</v>
-      </c>
-      <c r="I10" s="34"/>
-      <c r="J10" s="35"/>
-      <c r="K10" s="35"/>
-      <c r="L10" s="35"/>
-      <c r="M10" s="35"/>
-      <c r="N10" s="35"/>
-      <c r="O10" s="35"/>
-      <c r="Q10" s="36"/>
-      <c r="R10" s="37"/>
-    </row>
-    <row r="11" spans="1:24" s="33" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="33" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" s="33" t="s">
+      <c r="H10" s="1">
+        <v>0</v>
+      </c>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3"/>
+      <c r="Q10" s="4"/>
+      <c r="R10" s="2"/>
+    </row>
+    <row r="11" spans="1:24">
+      <c r="B11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D11" s="33" t="s">
+      <c r="D11" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="E11" s="33" t="s">
-        <v>2</v>
-      </c>
-      <c r="F11" s="33" t="s">
+      <c r="E11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H11" s="33">
-        <v>0</v>
-      </c>
-      <c r="I11" s="34"/>
-      <c r="J11" s="35"/>
-      <c r="K11" s="35"/>
-      <c r="L11" s="35"/>
-      <c r="M11" s="35"/>
-      <c r="N11" s="35"/>
-      <c r="O11" s="35"/>
-      <c r="Q11" s="36"/>
-      <c r="R11" s="37"/>
-    </row>
-    <row r="12" spans="1:24" s="33" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="33" t="s">
-        <v>25</v>
-      </c>
-      <c r="C12" s="33" t="s">
+      <c r="H11" s="1">
+        <v>0</v>
+      </c>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
+      <c r="Q11" s="4"/>
+      <c r="R11" s="2"/>
+    </row>
+    <row r="12" spans="1:24">
+      <c r="B12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D12" s="33" t="s">
+      <c r="D12" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="E12" s="33" t="s">
-        <v>2</v>
-      </c>
-      <c r="F12" s="33" t="s">
+      <c r="E12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="H12" s="33" t="b">
-        <v>0</v>
-      </c>
-      <c r="I12" s="34"/>
-      <c r="J12" s="35"/>
-      <c r="K12" s="35"/>
-      <c r="L12" s="35"/>
-      <c r="M12" s="35"/>
-      <c r="N12" s="35"/>
-      <c r="O12" s="35"/>
-      <c r="Q12" s="36"/>
-      <c r="R12" s="37"/>
-    </row>
-    <row r="13" spans="1:24" s="33" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="33" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13" s="33" t="s">
+      <c r="H12" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="3"/>
+      <c r="Q12" s="4"/>
+      <c r="R12" s="2"/>
+    </row>
+    <row r="13" spans="1:24">
+      <c r="B13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="D13" s="33" t="s">
+      <c r="D13" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="E13" s="33" t="s">
-        <v>2</v>
-      </c>
-      <c r="F13" s="33" t="s">
+      <c r="E13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F13" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H13" s="33">
+      <c r="H13" s="1">
         <v>15</v>
       </c>
-      <c r="I13" s="34"/>
-      <c r="J13" s="35"/>
-      <c r="K13" s="35"/>
-      <c r="L13" s="35"/>
-      <c r="M13" s="35"/>
-      <c r="N13" s="35"/>
-      <c r="O13" s="35"/>
-      <c r="Q13" s="36"/>
-      <c r="R13" s="37"/>
-    </row>
-    <row r="14" spans="1:24" s="33" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="33" t="s">
-        <v>25</v>
-      </c>
-      <c r="C14" s="33" t="s">
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="3"/>
+      <c r="N13" s="3"/>
+      <c r="O13" s="3"/>
+      <c r="Q13" s="4"/>
+      <c r="R13" s="2"/>
+    </row>
+    <row r="14" spans="1:24">
+      <c r="B14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="D14" s="33" t="s">
+      <c r="D14" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="E14" s="33" t="s">
-        <v>2</v>
-      </c>
-      <c r="F14" s="33" t="s">
+      <c r="E14" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F14" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="H14" s="33">
-        <v>0</v>
-      </c>
-      <c r="I14" s="34"/>
-      <c r="J14" s="35"/>
-      <c r="K14" s="35"/>
-      <c r="L14" s="35"/>
-      <c r="M14" s="35"/>
-      <c r="N14" s="35"/>
-      <c r="O14" s="35"/>
-      <c r="Q14" s="36"/>
-      <c r="R14" s="37"/>
-    </row>
-    <row r="15" spans="1:24" s="33" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="33" t="s">
-        <v>25</v>
-      </c>
-      <c r="C15" s="33" t="s">
+      <c r="H14" s="1">
+        <v>0</v>
+      </c>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
+      <c r="O14" s="3"/>
+      <c r="Q14" s="4"/>
+      <c r="R14" s="2"/>
+    </row>
+    <row r="15" spans="1:24">
+      <c r="B15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="D15" s="33" t="s">
+      <c r="D15" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="E15" s="33" t="s">
-        <v>2</v>
-      </c>
-      <c r="F15" s="33" t="s">
+      <c r="E15" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F15" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H15" s="33">
+      <c r="H15" s="1">
         <v>1</v>
       </c>
-      <c r="I15" s="34"/>
-      <c r="J15" s="35"/>
-      <c r="K15" s="35"/>
-      <c r="L15" s="35"/>
-      <c r="M15" s="35"/>
-      <c r="N15" s="35"/>
-      <c r="O15" s="35"/>
-      <c r="Q15" s="36"/>
-      <c r="R15" s="37"/>
-    </row>
-    <row r="16" spans="1:24" s="33" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="33" t="b">
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
+      <c r="M15" s="3"/>
+      <c r="N15" s="3"/>
+      <c r="O15" s="3"/>
+      <c r="Q15" s="4"/>
+      <c r="R15" s="2"/>
+    </row>
+    <row r="16" spans="1:24">
+      <c r="A16" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="B16" s="33" t="s">
+      <c r="B16" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C16" s="33" t="s">
+      <c r="C16" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="D16" s="33" t="s">
+      <c r="D16" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="I16" s="34"/>
-    </row>
-    <row r="17" spans="1:16" s="33" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="33" t="s">
+      <c r="H16" s="1"/>
+    </row>
+    <row r="17" spans="1:16">
+      <c r="B17" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C17" s="33" t="s">
+      <c r="C17" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="D17" s="33" t="s">
+      <c r="D17" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="E17" s="33" t="s">
+      <c r="E17" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F17" s="33" t="s">
+      <c r="F17" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="H17" s="33">
+      <c r="H17" s="1">
         <v>90</v>
       </c>
-      <c r="I17" s="34"/>
-      <c r="J17" s="33">
-        <v>0</v>
-      </c>
-      <c r="K17" s="33">
+      <c r="J17" s="1">
+        <v>0</v>
+      </c>
+      <c r="K17" s="1">
         <v>359</v>
       </c>
-      <c r="L17" s="33">
+      <c r="L17" s="1">
         <v>180</v>
       </c>
-      <c r="M17" s="35">
+      <c r="M17" s="3">
         <f>(K17-J17)/6</f>
         <v>59.833333333333336</v>
       </c>
-      <c r="N17" s="35"/>
-      <c r="O17" s="35"/>
-      <c r="P17" s="33" t="s">
+      <c r="N17" s="3"/>
+      <c r="O17" s="3"/>
+      <c r="P17" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:16" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A18" s="20" t="b">
+    <row r="18" spans="1:16" ht="15">
+      <c r="A18" s="34" t="b">
         <v>1</v>
       </c>
-      <c r="B18" s="20" t="s">
+      <c r="B18" s="34" t="s">
         <v>266</v>
       </c>
-      <c r="C18" s="20" t="s">
+      <c r="C18" s="34" t="s">
         <v>267</v>
       </c>
-      <c r="D18" s="20" t="s">
+      <c r="D18" s="34" t="s">
         <v>76</v>
       </c>
-      <c r="E18" s="20"/>
-      <c r="F18" s="20"/>
-      <c r="G18" s="20"/>
-      <c r="H18" s="20"/>
-      <c r="I18" s="20"/>
-    </row>
-    <row r="19" spans="1:16" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E18" s="34"/>
+      <c r="F18" s="34"/>
+      <c r="G18" s="34"/>
+      <c r="H18" s="34"/>
+      <c r="I18" s="34"/>
+    </row>
+    <row r="19" spans="1:16" customFormat="1" ht="15">
       <c r="A19" s="20"/>
       <c r="B19" s="20" t="s">
         <v>26</v>
       </c>
       <c r="C19" s="20" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="D19" s="20" t="s">
         <v>269</v>
@@ -5730,7 +5701,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="20" spans="1:16" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:16" customFormat="1" ht="15">
       <c r="A20" s="20"/>
       <c r="B20" s="20" t="s">
         <v>25</v>
@@ -5753,7 +5724,7 @@
       </c>
       <c r="I20" s="20"/>
     </row>
-    <row r="21" spans="1:16" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:16" customFormat="1" ht="15">
       <c r="A21" s="20"/>
       <c r="B21" s="20" t="s">
         <v>25</v>
@@ -5776,7 +5747,7 @@
       </c>
       <c r="I21" s="20"/>
     </row>
-    <row r="22" spans="1:16" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:16" customFormat="1" ht="15">
       <c r="A22" s="20"/>
       <c r="B22" s="20" t="s">
         <v>25</v>
@@ -5799,7 +5770,7 @@
       </c>
       <c r="I22" s="20"/>
     </row>
-    <row r="23" spans="1:16" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:16" customFormat="1" ht="15">
       <c r="A23" s="20" t="b">
         <v>1</v>
       </c>
@@ -5818,13 +5789,13 @@
       <c r="H23" s="20"/>
       <c r="I23" s="20"/>
     </row>
-    <row r="24" spans="1:16" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:16" customFormat="1" ht="15">
       <c r="A24" s="20"/>
       <c r="B24" s="20" t="s">
         <v>26</v>
       </c>
       <c r="C24" s="20" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="D24" s="20" t="s">
         <v>269</v>
@@ -5840,17 +5811,24 @@
         <v>30</v>
       </c>
       <c r="I24" s="20"/>
-      <c r="N24" t="s">
-        <v>519</v>
-      </c>
-      <c r="O24" t="s">
-        <v>520</v>
+      <c r="J24">
+        <v>0</v>
+      </c>
+      <c r="K24">
+        <v>100</v>
+      </c>
+      <c r="L24" s="20">
+        <v>50</v>
+      </c>
+      <c r="M24" s="3">
+        <f>(K24-J24)/6</f>
+        <v>16.666666666666668</v>
       </c>
       <c r="P24" t="s">
-        <v>521</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" customFormat="1" ht="15">
       <c r="A25" s="20"/>
       <c r="B25" s="20" t="s">
         <v>25</v>
@@ -5873,7 +5851,7 @@
       </c>
       <c r="I25" s="20"/>
     </row>
-    <row r="26" spans="1:16" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:16" customFormat="1" ht="15">
       <c r="A26" s="20"/>
       <c r="B26" s="20" t="s">
         <v>25</v>
@@ -5896,7 +5874,7 @@
       </c>
       <c r="I26" s="20"/>
     </row>
-    <row r="27" spans="1:16" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:16" customFormat="1" ht="15">
       <c r="A27" s="20"/>
       <c r="B27" s="20" t="s">
         <v>25</v>
@@ -5919,7 +5897,7 @@
       </c>
       <c r="I27" s="20"/>
     </row>
-    <row r="28" spans="1:16" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:16" customFormat="1" ht="15">
       <c r="A28" s="20" t="b">
         <v>1</v>
       </c>
@@ -5938,7 +5916,7 @@
       <c r="H28" s="20"/>
       <c r="I28" s="20"/>
     </row>
-    <row r="29" spans="1:16" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:16" customFormat="1" ht="15">
       <c r="A29" s="20"/>
       <c r="B29" s="20" t="s">
         <v>26</v>
@@ -5977,7 +5955,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:16" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:16" customFormat="1" ht="15">
       <c r="A30" s="20"/>
       <c r="B30" s="20" t="s">
         <v>25</v>
@@ -6000,7 +5978,7 @@
       </c>
       <c r="I30" s="20"/>
     </row>
-    <row r="31" spans="1:16" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:16" customFormat="1" ht="15">
       <c r="A31" s="20"/>
       <c r="B31" s="20" t="s">
         <v>25</v>
@@ -6025,7 +6003,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="32" spans="1:16" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:16" customFormat="1" ht="15">
       <c r="A32" s="20" t="b">
         <v>1</v>
       </c>
@@ -6044,7 +6022,7 @@
       <c r="H32" s="20"/>
       <c r="I32" s="20"/>
     </row>
-    <row r="33" spans="1:9" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" customFormat="1" ht="15">
       <c r="A33" s="20"/>
       <c r="B33" s="20" t="s">
         <v>25</v>
@@ -6069,7 +6047,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="34" spans="1:9" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" customFormat="1" ht="15">
       <c r="A34" s="20"/>
       <c r="B34" s="20" t="s">
         <v>25</v>
@@ -6118,21 +6096,21 @@
       <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="29.44140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="28.77734375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.44140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="14.44140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="14.77734375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="29.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="28.83203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5" style="1" customWidth="1"/>
+    <col min="5" max="5" width="14.83203125" style="1" customWidth="1"/>
     <col min="6" max="6" width="9.6640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.44140625" style="1"/>
+    <col min="7" max="7" width="11.5" style="1"/>
     <col min="8" max="8" width="14" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.44140625" style="5"/>
-    <col min="10" max="16384" width="11.44140625" style="1"/>
+    <col min="9" max="9" width="11.5" style="5"/>
+    <col min="10" max="16384" width="11.5" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="18">
       <c r="A1" s="6"/>
       <c r="B1" s="6"/>
       <c r="C1" s="8" t="s">
@@ -6145,7 +6123,7 @@
       <c r="H1" s="7"/>
       <c r="I1" s="7"/>
     </row>
-    <row r="2" spans="1:9" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" s="9" customFormat="1" ht="15">
       <c r="A2" s="9" t="s">
         <v>485</v>
       </c>
@@ -6164,7 +6142,7 @@
       <c r="H2" s="10"/>
       <c r="I2" s="10"/>
     </row>
-    <row r="3" spans="1:9" s="16" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" s="16" customFormat="1" ht="15">
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>
       <c r="D3" s="11" t="s">
@@ -6178,7 +6156,7 @@
       <c r="H3" s="11"/>
       <c r="I3" s="11"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
         <v>499</v>
       </c>
@@ -6198,7 +6176,7 @@
       <c r="G4"/>
       <c r="H4"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
         <v>502</v>
       </c>
@@ -6219,7 +6197,7 @@
       <c r="H5"/>
       <c r="I5"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9">
       <c r="A6"/>
       <c r="B6"/>
       <c r="C6"/>
@@ -6229,7 +6207,7 @@
       <c r="G6"/>
       <c r="H6"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9">
       <c r="A7"/>
       <c r="B7"/>
       <c r="C7"/>
@@ -6240,7 +6218,7 @@
       <c r="H7"/>
       <c r="I7"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9">
       <c r="A8"/>
       <c r="B8"/>
       <c r="C8"/>
@@ -6250,7 +6228,7 @@
       <c r="G8"/>
       <c r="H8"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9">
       <c r="A9"/>
       <c r="B9"/>
       <c r="C9" s="15"/>
@@ -6260,7 +6238,7 @@
       <c r="G9"/>
       <c r="H9"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9">
       <c r="A10"/>
       <c r="B10"/>
       <c r="C10"/>
@@ -6270,7 +6248,7 @@
       <c r="G10"/>
       <c r="H10"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9">
       <c r="A11"/>
       <c r="B11"/>
       <c r="C11"/>
@@ -6280,7 +6258,7 @@
       <c r="G11"/>
       <c r="H11"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9">
       <c r="A12"/>
       <c r="B12"/>
       <c r="C12"/>
@@ -6290,7 +6268,7 @@
       <c r="G12"/>
       <c r="H12"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9">
       <c r="A13"/>
       <c r="B13"/>
       <c r="C13"/>
@@ -6300,7 +6278,7 @@
       <c r="G13"/>
       <c r="H13"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9">
       <c r="A14"/>
       <c r="B14"/>
       <c r="C14"/>
@@ -6310,7 +6288,7 @@
       <c r="G14"/>
       <c r="H14"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9">
       <c r="A15"/>
       <c r="B15"/>
       <c r="C15"/>
@@ -6320,15 +6298,15 @@
       <c r="G15"/>
       <c r="H15"/>
     </row>
-    <row r="16" spans="1:9" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="17" spans="1:9" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="18" spans="1:9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" customFormat="1"/>
+    <row r="17" spans="1:9" customFormat="1"/>
+    <row r="18" spans="1:9" customFormat="1">
       <c r="C18" s="19"/>
     </row>
-    <row r="19" spans="1:9" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="20" spans="1:9" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="21" spans="1:9" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" customFormat="1"/>
+    <row r="20" spans="1:9" customFormat="1"/>
+    <row r="21" spans="1:9" customFormat="1"/>
+    <row r="22" spans="1:9">
       <c r="A22"/>
       <c r="B22"/>
       <c r="C22"/>
@@ -6338,7 +6316,7 @@
       <c r="G22"/>
       <c r="H22"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9">
       <c r="A23"/>
       <c r="B23"/>
       <c r="C23"/>
@@ -6348,7 +6326,7 @@
       <c r="G23"/>
       <c r="H23"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9">
       <c r="A24"/>
       <c r="B24"/>
       <c r="C24"/>
@@ -6358,7 +6336,7 @@
       <c r="G24"/>
       <c r="H24"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9">
       <c r="A25"/>
       <c r="B25"/>
       <c r="C25"/>
@@ -6368,7 +6346,7 @@
       <c r="G25"/>
       <c r="H25"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9">
       <c r="A26"/>
       <c r="B26"/>
       <c r="C26"/>
@@ -6378,7 +6356,7 @@
       <c r="G26"/>
       <c r="H26"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9">
       <c r="A27"/>
       <c r="B27"/>
       <c r="C27"/>
@@ -6389,7 +6367,7 @@
       <c r="H27"/>
       <c r="I27"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9">
       <c r="A28"/>
       <c r="B28"/>
       <c r="C28"/>
@@ -6399,7 +6377,7 @@
       <c r="G28"/>
       <c r="H28"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9">
       <c r="A29"/>
       <c r="B29"/>
       <c r="C29"/>
@@ -6409,7 +6387,7 @@
       <c r="G29"/>
       <c r="H29"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9">
       <c r="A30"/>
       <c r="B30"/>
       <c r="C30"/>
@@ -6419,7 +6397,7 @@
       <c r="G30"/>
       <c r="H30"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9">
       <c r="A31"/>
       <c r="B31"/>
       <c r="C31"/>
@@ -6445,23 +6423,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I327"/>
   <sheetViews>
-    <sheetView topLeftCell="A299" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="A299" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
       <selection activeCell="A325" sqref="A325:XFD327"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="70.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="80.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="70.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="80.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.1640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="33.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="255.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="255.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="15">
       <c r="A1" s="20" t="b">
         <v>0</v>
       </c>
@@ -6480,7 +6458,7 @@
       <c r="H1" s="20"/>
       <c r="I1" s="20"/>
     </row>
-    <row r="2" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="15">
       <c r="A2" s="20"/>
       <c r="B2" s="20" t="s">
         <v>25</v>
@@ -6501,7 +6479,7 @@
       <c r="H2" s="20"/>
       <c r="I2" s="20"/>
     </row>
-    <row r="3" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="15">
       <c r="A3" s="20"/>
       <c r="B3" s="20" t="s">
         <v>25</v>
@@ -6524,7 +6502,7 @@
       </c>
       <c r="I3" s="20"/>
     </row>
-    <row r="4" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="15">
       <c r="A4" s="20"/>
       <c r="B4" s="20" t="s">
         <v>25</v>
@@ -6547,7 +6525,7 @@
       </c>
       <c r="I4" s="20"/>
     </row>
-    <row r="5" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="15">
       <c r="A5" s="20"/>
       <c r="B5" s="20" t="s">
         <v>25</v>
@@ -6570,7 +6548,7 @@
       </c>
       <c r="I5" s="20"/>
     </row>
-    <row r="6" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="15">
       <c r="A6" s="20"/>
       <c r="B6" s="20" t="s">
         <v>25</v>
@@ -6593,7 +6571,7 @@
       </c>
       <c r="I6" s="20"/>
     </row>
-    <row r="7" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="15">
       <c r="A7" s="20"/>
       <c r="B7" s="20" t="s">
         <v>25</v>
@@ -6616,7 +6594,7 @@
       </c>
       <c r="I7" s="20"/>
     </row>
-    <row r="8" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="15">
       <c r="A8" s="20"/>
       <c r="B8" s="20" t="s">
         <v>25</v>
@@ -6639,7 +6617,7 @@
       </c>
       <c r="I8" s="20"/>
     </row>
-    <row r="9" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="15">
       <c r="A9" s="20"/>
       <c r="B9" s="20" t="s">
         <v>25</v>
@@ -6662,7 +6640,7 @@
       </c>
       <c r="I9" s="20"/>
     </row>
-    <row r="10" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="15">
       <c r="A10" s="20"/>
       <c r="B10" s="20" t="s">
         <v>25</v>
@@ -6685,7 +6663,7 @@
       </c>
       <c r="I10" s="20"/>
     </row>
-    <row r="11" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="15">
       <c r="A11" s="20" t="b">
         <v>0</v>
       </c>
@@ -6704,7 +6682,7 @@
       <c r="H11" s="20"/>
       <c r="I11" s="20"/>
     </row>
-    <row r="12" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="15">
       <c r="A12" s="20"/>
       <c r="B12" s="20" t="s">
         <v>25</v>
@@ -6725,7 +6703,7 @@
       <c r="H12" s="20"/>
       <c r="I12" s="20"/>
     </row>
-    <row r="13" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" ht="15">
       <c r="A13" s="20"/>
       <c r="B13" s="20" t="s">
         <v>25</v>
@@ -6748,7 +6726,7 @@
       </c>
       <c r="I13" s="20"/>
     </row>
-    <row r="14" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="15">
       <c r="A14" s="20"/>
       <c r="B14" s="20" t="s">
         <v>25</v>
@@ -6771,7 +6749,7 @@
       </c>
       <c r="I14" s="20"/>
     </row>
-    <row r="15" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="15">
       <c r="A15" s="20"/>
       <c r="B15" s="20" t="s">
         <v>25</v>
@@ -6794,7 +6772,7 @@
       </c>
       <c r="I15" s="20"/>
     </row>
-    <row r="16" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" ht="15">
       <c r="A16" s="20"/>
       <c r="B16" s="20" t="s">
         <v>25</v>
@@ -6817,7 +6795,7 @@
       </c>
       <c r="I16" s="20"/>
     </row>
-    <row r="17" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" ht="15">
       <c r="A17" s="20"/>
       <c r="B17" s="20" t="s">
         <v>25</v>
@@ -6840,7 +6818,7 @@
       </c>
       <c r="I17" s="20"/>
     </row>
-    <row r="18" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" ht="15">
       <c r="A18" s="20"/>
       <c r="B18" s="20" t="s">
         <v>25</v>
@@ -6863,7 +6841,7 @@
       </c>
       <c r="I18" s="20"/>
     </row>
-    <row r="19" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" ht="15">
       <c r="A19" s="20"/>
       <c r="B19" s="20" t="s">
         <v>25</v>
@@ -6886,7 +6864,7 @@
       </c>
       <c r="I19" s="20"/>
     </row>
-    <row r="20" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" ht="15">
       <c r="A20" s="20"/>
       <c r="B20" s="20" t="s">
         <v>25</v>
@@ -6909,7 +6887,7 @@
       </c>
       <c r="I20" s="20"/>
     </row>
-    <row r="21" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" ht="15">
       <c r="A21" s="20" t="b">
         <v>0</v>
       </c>
@@ -6928,7 +6906,7 @@
       <c r="H21" s="20"/>
       <c r="I21" s="20"/>
     </row>
-    <row r="22" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" ht="15">
       <c r="A22" s="20"/>
       <c r="B22" s="20" t="s">
         <v>25</v>
@@ -6951,7 +6929,7 @@
       </c>
       <c r="I22" s="20"/>
     </row>
-    <row r="23" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" ht="15">
       <c r="A23" s="20"/>
       <c r="B23" s="20" t="s">
         <v>25</v>
@@ -6974,7 +6952,7 @@
       </c>
       <c r="I23" s="20"/>
     </row>
-    <row r="24" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" ht="15">
       <c r="A24" s="20"/>
       <c r="B24" s="20" t="s">
         <v>25</v>
@@ -6997,7 +6975,7 @@
       </c>
       <c r="I24" s="20"/>
     </row>
-    <row r="25" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" ht="15">
       <c r="A25" s="20"/>
       <c r="B25" s="20" t="s">
         <v>25</v>
@@ -7020,7 +6998,7 @@
       </c>
       <c r="I25" s="20"/>
     </row>
-    <row r="26" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" ht="15">
       <c r="A26" s="20"/>
       <c r="B26" s="20" t="s">
         <v>25</v>
@@ -7043,7 +7021,7 @@
       </c>
       <c r="I26" s="20"/>
     </row>
-    <row r="27" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" ht="15">
       <c r="A27" s="20"/>
       <c r="B27" s="20" t="s">
         <v>25</v>
@@ -7066,7 +7044,7 @@
       </c>
       <c r="I27" s="20"/>
     </row>
-    <row r="28" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" ht="15">
       <c r="A28" s="20"/>
       <c r="B28" s="20" t="s">
         <v>25</v>
@@ -7089,7 +7067,7 @@
       </c>
       <c r="I28" s="20"/>
     </row>
-    <row r="29" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" ht="15">
       <c r="A29" s="20"/>
       <c r="B29" s="20" t="s">
         <v>25</v>
@@ -7112,7 +7090,7 @@
       </c>
       <c r="I29" s="20"/>
     </row>
-    <row r="30" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" ht="15">
       <c r="A30" s="20"/>
       <c r="B30" s="20" t="s">
         <v>25</v>
@@ -7135,7 +7113,7 @@
       </c>
       <c r="I30" s="20"/>
     </row>
-    <row r="31" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" ht="15">
       <c r="A31" s="20" t="b">
         <v>0</v>
       </c>
@@ -7154,7 +7132,7 @@
       <c r="H31" s="20"/>
       <c r="I31" s="20"/>
     </row>
-    <row r="32" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" ht="15">
       <c r="A32" s="20"/>
       <c r="B32" s="20" t="s">
         <v>25</v>
@@ -7175,7 +7153,7 @@
       <c r="H32" s="20"/>
       <c r="I32" s="20"/>
     </row>
-    <row r="33" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" ht="15">
       <c r="A33" s="20"/>
       <c r="B33" s="20" t="s">
         <v>25</v>
@@ -7198,7 +7176,7 @@
       </c>
       <c r="I33" s="20"/>
     </row>
-    <row r="34" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" ht="15">
       <c r="A34" s="20"/>
       <c r="B34" s="20" t="s">
         <v>25</v>
@@ -7221,7 +7199,7 @@
       </c>
       <c r="I34" s="20"/>
     </row>
-    <row r="35" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" ht="15">
       <c r="A35" s="20"/>
       <c r="B35" s="20" t="s">
         <v>25</v>
@@ -7244,7 +7222,7 @@
       </c>
       <c r="I35" s="20"/>
     </row>
-    <row r="36" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" ht="15">
       <c r="A36" s="20"/>
       <c r="B36" s="20" t="s">
         <v>25</v>
@@ -7267,7 +7245,7 @@
       </c>
       <c r="I36" s="20"/>
     </row>
-    <row r="37" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" ht="15">
       <c r="A37" s="20"/>
       <c r="B37" s="20" t="s">
         <v>25</v>
@@ -7290,7 +7268,7 @@
       </c>
       <c r="I37" s="20"/>
     </row>
-    <row r="38" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" ht="15">
       <c r="A38" s="20"/>
       <c r="B38" s="20" t="s">
         <v>25</v>
@@ -7313,7 +7291,7 @@
       </c>
       <c r="I38" s="20"/>
     </row>
-    <row r="39" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" ht="15">
       <c r="A39" s="20"/>
       <c r="B39" s="20" t="s">
         <v>25</v>
@@ -7336,7 +7314,7 @@
       </c>
       <c r="I39" s="20"/>
     </row>
-    <row r="40" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" ht="15">
       <c r="A40" s="20"/>
       <c r="B40" s="20" t="s">
         <v>25</v>
@@ -7359,7 +7337,7 @@
       </c>
       <c r="I40" s="20"/>
     </row>
-    <row r="41" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" ht="15">
       <c r="A41" s="20" t="b">
         <v>0</v>
       </c>
@@ -7378,7 +7356,7 @@
       <c r="H41" s="20"/>
       <c r="I41" s="20"/>
     </row>
-    <row r="42" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" ht="15">
       <c r="A42" s="20"/>
       <c r="B42" s="20" t="s">
         <v>25</v>
@@ -7399,7 +7377,7 @@
       <c r="H42" s="20"/>
       <c r="I42" s="20"/>
     </row>
-    <row r="43" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" ht="15">
       <c r="A43" s="20"/>
       <c r="B43" s="20" t="s">
         <v>25</v>
@@ -7422,7 +7400,7 @@
       </c>
       <c r="I43" s="20"/>
     </row>
-    <row r="44" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" ht="15">
       <c r="A44" s="20"/>
       <c r="B44" s="20" t="s">
         <v>25</v>
@@ -7445,7 +7423,7 @@
       </c>
       <c r="I44" s="20"/>
     </row>
-    <row r="45" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" ht="15">
       <c r="A45" s="20"/>
       <c r="B45" s="20" t="s">
         <v>25</v>
@@ -7468,7 +7446,7 @@
       </c>
       <c r="I45" s="20"/>
     </row>
-    <row r="46" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" ht="15">
       <c r="A46" s="20"/>
       <c r="B46" s="20" t="s">
         <v>25</v>
@@ -7491,7 +7469,7 @@
       </c>
       <c r="I46" s="20"/>
     </row>
-    <row r="47" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" ht="15">
       <c r="A47" s="20"/>
       <c r="B47" s="20" t="s">
         <v>25</v>
@@ -7514,7 +7492,7 @@
       </c>
       <c r="I47" s="20"/>
     </row>
-    <row r="48" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" ht="15">
       <c r="A48" s="20"/>
       <c r="B48" s="20" t="s">
         <v>25</v>
@@ -7537,7 +7515,7 @@
       </c>
       <c r="I48" s="20"/>
     </row>
-    <row r="49" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" ht="15">
       <c r="A49" s="20"/>
       <c r="B49" s="20" t="s">
         <v>25</v>
@@ -7560,7 +7538,7 @@
       </c>
       <c r="I49" s="20"/>
     </row>
-    <row r="50" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" ht="15">
       <c r="A50" s="20"/>
       <c r="B50" s="20" t="s">
         <v>25</v>
@@ -7583,7 +7561,7 @@
       </c>
       <c r="I50" s="20"/>
     </row>
-    <row r="51" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" ht="15">
       <c r="A51" s="20" t="b">
         <v>0</v>
       </c>
@@ -7602,7 +7580,7 @@
       <c r="H51" s="20"/>
       <c r="I51" s="20"/>
     </row>
-    <row r="52" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" ht="15">
       <c r="A52" s="20"/>
       <c r="B52" s="20" t="s">
         <v>25</v>
@@ -7623,7 +7601,7 @@
       <c r="H52" s="20"/>
       <c r="I52" s="20"/>
     </row>
-    <row r="53" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:9" ht="15">
       <c r="A53" s="20"/>
       <c r="B53" s="20" t="s">
         <v>25</v>
@@ -7646,7 +7624,7 @@
       </c>
       <c r="I53" s="20"/>
     </row>
-    <row r="54" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9" ht="15">
       <c r="A54" s="20"/>
       <c r="B54" s="20" t="s">
         <v>25</v>
@@ -7669,7 +7647,7 @@
       </c>
       <c r="I54" s="20"/>
     </row>
-    <row r="55" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:9" ht="15">
       <c r="A55" s="20"/>
       <c r="B55" s="20" t="s">
         <v>25</v>
@@ -7692,7 +7670,7 @@
       </c>
       <c r="I55" s="20"/>
     </row>
-    <row r="56" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:9" ht="15">
       <c r="A56" s="20"/>
       <c r="B56" s="20" t="s">
         <v>25</v>
@@ -7715,7 +7693,7 @@
       </c>
       <c r="I56" s="20"/>
     </row>
-    <row r="57" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:9" ht="15">
       <c r="A57" s="20"/>
       <c r="B57" s="20" t="s">
         <v>25</v>
@@ -7738,7 +7716,7 @@
       </c>
       <c r="I57" s="20"/>
     </row>
-    <row r="58" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:9" ht="15">
       <c r="A58" s="20"/>
       <c r="B58" s="20" t="s">
         <v>25</v>
@@ -7761,7 +7739,7 @@
       </c>
       <c r="I58" s="20"/>
     </row>
-    <row r="59" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:9" ht="15">
       <c r="A59" s="20"/>
       <c r="B59" s="20" t="s">
         <v>25</v>
@@ -7784,7 +7762,7 @@
       </c>
       <c r="I59" s="20"/>
     </row>
-    <row r="60" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:9" ht="15">
       <c r="A60" s="20"/>
       <c r="B60" s="20" t="s">
         <v>25</v>
@@ -7807,7 +7785,7 @@
       </c>
       <c r="I60" s="20"/>
     </row>
-    <row r="61" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:9" ht="15">
       <c r="A61" s="20" t="b">
         <v>0</v>
       </c>
@@ -7826,7 +7804,7 @@
       <c r="H61" s="20"/>
       <c r="I61" s="20"/>
     </row>
-    <row r="62" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:9" ht="15">
       <c r="A62" s="20"/>
       <c r="B62" s="20" t="s">
         <v>25</v>
@@ -7847,7 +7825,7 @@
       <c r="H62" s="20"/>
       <c r="I62" s="20"/>
     </row>
-    <row r="63" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:9" ht="15">
       <c r="A63" s="20"/>
       <c r="B63" s="20" t="s">
         <v>25</v>
@@ -7872,7 +7850,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="64" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:9" ht="15">
       <c r="A64" s="20"/>
       <c r="B64" s="20" t="s">
         <v>25</v>
@@ -7895,7 +7873,7 @@
       </c>
       <c r="I64" s="20"/>
     </row>
-    <row r="65" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:9" ht="15">
       <c r="A65" s="20"/>
       <c r="B65" s="20" t="s">
         <v>25</v>
@@ -7918,7 +7896,7 @@
       </c>
       <c r="I65" s="20"/>
     </row>
-    <row r="66" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:9" ht="15">
       <c r="A66" s="20"/>
       <c r="B66" s="20" t="s">
         <v>25</v>
@@ -7941,7 +7919,7 @@
       </c>
       <c r="I66" s="20"/>
     </row>
-    <row r="67" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:9" ht="15">
       <c r="A67" s="20"/>
       <c r="B67" s="20" t="s">
         <v>25</v>
@@ -7964,7 +7942,7 @@
       </c>
       <c r="I67" s="20"/>
     </row>
-    <row r="68" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:9" ht="15">
       <c r="A68" s="20"/>
       <c r="B68" s="20" t="s">
         <v>25</v>
@@ -7987,7 +7965,7 @@
       </c>
       <c r="I68" s="20"/>
     </row>
-    <row r="69" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:9" ht="15">
       <c r="A69" s="20"/>
       <c r="B69" s="20" t="s">
         <v>25</v>
@@ -8010,7 +7988,7 @@
       </c>
       <c r="I69" s="20"/>
     </row>
-    <row r="70" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:9" ht="15">
       <c r="A70" s="20"/>
       <c r="B70" s="20" t="s">
         <v>25</v>
@@ -8033,7 +8011,7 @@
       </c>
       <c r="I70" s="20"/>
     </row>
-    <row r="71" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:9" ht="15">
       <c r="A71" s="20"/>
       <c r="B71" s="20" t="s">
         <v>25</v>
@@ -8056,7 +8034,7 @@
       </c>
       <c r="I71" s="20"/>
     </row>
-    <row r="72" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:9" ht="15">
       <c r="A72" s="20" t="b">
         <v>0</v>
       </c>
@@ -8075,7 +8053,7 @@
       <c r="H72" s="20"/>
       <c r="I72" s="20"/>
     </row>
-    <row r="73" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:9" ht="15">
       <c r="A73" s="20"/>
       <c r="B73" s="20" t="s">
         <v>25</v>
@@ -8096,7 +8074,7 @@
       <c r="H73" s="20"/>
       <c r="I73" s="20"/>
     </row>
-    <row r="74" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:9" ht="15">
       <c r="A74" s="20"/>
       <c r="B74" s="20" t="s">
         <v>25</v>
@@ -8119,7 +8097,7 @@
       </c>
       <c r="I74" s="20"/>
     </row>
-    <row r="75" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:9" ht="15">
       <c r="A75" s="20"/>
       <c r="B75" s="20" t="s">
         <v>25</v>
@@ -8144,7 +8122,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="76" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:9" ht="15">
       <c r="A76" s="20"/>
       <c r="B76" s="20" t="s">
         <v>25</v>
@@ -8167,7 +8145,7 @@
       </c>
       <c r="I76" s="20"/>
     </row>
-    <row r="77" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:9" ht="15">
       <c r="A77" s="20"/>
       <c r="B77" s="20" t="s">
         <v>25</v>
@@ -8190,7 +8168,7 @@
       </c>
       <c r="I77" s="20"/>
     </row>
-    <row r="78" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:9" ht="15">
       <c r="A78" s="20"/>
       <c r="B78" s="20" t="s">
         <v>25</v>
@@ -8213,7 +8191,7 @@
       </c>
       <c r="I78" s="20"/>
     </row>
-    <row r="79" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:9" ht="15">
       <c r="A79" s="20"/>
       <c r="B79" s="20" t="s">
         <v>25</v>
@@ -8236,7 +8214,7 @@
       </c>
       <c r="I79" s="20"/>
     </row>
-    <row r="80" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:9" ht="15">
       <c r="A80" s="20"/>
       <c r="B80" s="20" t="s">
         <v>25</v>
@@ -8259,7 +8237,7 @@
       </c>
       <c r="I80" s="20"/>
     </row>
-    <row r="81" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:9" ht="15">
       <c r="A81" s="20"/>
       <c r="B81" s="20" t="s">
         <v>25</v>
@@ -8282,7 +8260,7 @@
       </c>
       <c r="I81" s="20"/>
     </row>
-    <row r="82" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:9" ht="15">
       <c r="A82" s="20"/>
       <c r="B82" s="20" t="s">
         <v>25</v>
@@ -8305,7 +8283,7 @@
       </c>
       <c r="I82" s="20"/>
     </row>
-    <row r="83" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:9" ht="15">
       <c r="A83" s="20"/>
       <c r="B83" s="20" t="s">
         <v>25</v>
@@ -8328,7 +8306,7 @@
       </c>
       <c r="I83" s="20"/>
     </row>
-    <row r="84" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:9" ht="15">
       <c r="A84" s="20"/>
       <c r="B84" s="20" t="s">
         <v>25</v>
@@ -8351,7 +8329,7 @@
       </c>
       <c r="I84" s="20"/>
     </row>
-    <row r="85" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:9" ht="15">
       <c r="A85" s="20"/>
       <c r="B85" s="20" t="s">
         <v>25</v>
@@ -8374,7 +8352,7 @@
       </c>
       <c r="I85" s="20"/>
     </row>
-    <row r="86" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:9" ht="15">
       <c r="A86" s="20" t="b">
         <v>0</v>
       </c>
@@ -8393,7 +8371,7 @@
       <c r="H86" s="20"/>
       <c r="I86" s="20"/>
     </row>
-    <row r="87" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:9" ht="15">
       <c r="A87" s="20"/>
       <c r="B87" s="20" t="s">
         <v>25</v>
@@ -8416,7 +8394,7 @@
       </c>
       <c r="I87" s="20"/>
     </row>
-    <row r="88" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:9" ht="15">
       <c r="A88" s="20"/>
       <c r="B88" s="20" t="s">
         <v>25</v>
@@ -8439,7 +8417,7 @@
       </c>
       <c r="I88" s="20"/>
     </row>
-    <row r="89" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:9" ht="15">
       <c r="A89" s="20"/>
       <c r="B89" s="20" t="s">
         <v>25</v>
@@ -8462,7 +8440,7 @@
       </c>
       <c r="I89" s="20"/>
     </row>
-    <row r="90" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:9" ht="15">
       <c r="A90" s="20"/>
       <c r="B90" s="20" t="s">
         <v>25</v>
@@ -8485,7 +8463,7 @@
       </c>
       <c r="I90" s="20"/>
     </row>
-    <row r="91" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:9" ht="15">
       <c r="A91" s="20"/>
       <c r="B91" s="20" t="s">
         <v>25</v>
@@ -8508,7 +8486,7 @@
       </c>
       <c r="I91" s="20"/>
     </row>
-    <row r="92" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:9" ht="15">
       <c r="A92" s="20"/>
       <c r="B92" s="20" t="s">
         <v>25</v>
@@ -8531,7 +8509,7 @@
       </c>
       <c r="I92" s="20"/>
     </row>
-    <row r="93" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:9" ht="15">
       <c r="A93" s="20"/>
       <c r="B93" s="20" t="s">
         <v>25</v>
@@ -8554,7 +8532,7 @@
       </c>
       <c r="I93" s="20"/>
     </row>
-    <row r="94" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:9" ht="15">
       <c r="A94" s="20"/>
       <c r="B94" s="20" t="s">
         <v>25</v>
@@ -8577,7 +8555,7 @@
       </c>
       <c r="I94" s="20"/>
     </row>
-    <row r="95" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:9" ht="15">
       <c r="A95" s="20"/>
       <c r="B95" s="20" t="s">
         <v>25</v>
@@ -8600,7 +8578,7 @@
       </c>
       <c r="I95" s="20"/>
     </row>
-    <row r="96" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:9" ht="15">
       <c r="A96" s="20"/>
       <c r="B96" s="20" t="s">
         <v>25</v>
@@ -8623,7 +8601,7 @@
       </c>
       <c r="I96" s="20"/>
     </row>
-    <row r="97" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:9" ht="15">
       <c r="A97" s="20" t="b">
         <v>0</v>
       </c>
@@ -8642,7 +8620,7 @@
       <c r="H97" s="20"/>
       <c r="I97" s="20"/>
     </row>
-    <row r="98" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:9" ht="15">
       <c r="A98" s="20"/>
       <c r="B98" s="20" t="s">
         <v>25</v>
@@ -8667,7 +8645,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="99" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:9" ht="15">
       <c r="A99" s="20" t="b">
         <v>0</v>
       </c>
@@ -8686,7 +8664,7 @@
       <c r="H99" s="20"/>
       <c r="I99" s="20"/>
     </row>
-    <row r="100" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:9" ht="15">
       <c r="A100" s="20"/>
       <c r="B100" s="20" t="s">
         <v>25</v>
@@ -8707,7 +8685,7 @@
       <c r="H100" s="20"/>
       <c r="I100" s="20"/>
     </row>
-    <row r="101" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:9" ht="15">
       <c r="A101" s="20"/>
       <c r="B101" s="20" t="s">
         <v>25</v>
@@ -8732,7 +8710,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="102" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:9" ht="15">
       <c r="A102" s="20" t="b">
         <v>0</v>
       </c>
@@ -8751,7 +8729,7 @@
       <c r="H102" s="20"/>
       <c r="I102" s="20"/>
     </row>
-    <row r="103" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:9" ht="15">
       <c r="A103" s="20"/>
       <c r="B103" s="20" t="s">
         <v>25</v>
@@ -8774,7 +8752,7 @@
       </c>
       <c r="I103" s="20"/>
     </row>
-    <row r="104" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:9" ht="15">
       <c r="A104" s="20"/>
       <c r="B104" s="20" t="s">
         <v>25</v>
@@ -8799,7 +8777,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="105" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:9" ht="15">
       <c r="A105" s="20"/>
       <c r="B105" s="20" t="s">
         <v>25</v>
@@ -8822,7 +8800,7 @@
       </c>
       <c r="I105" s="20"/>
     </row>
-    <row r="106" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:9" ht="15">
       <c r="A106" s="20"/>
       <c r="B106" s="20" t="s">
         <v>25</v>
@@ -8843,7 +8821,7 @@
       <c r="H106" s="20"/>
       <c r="I106" s="20"/>
     </row>
-    <row r="107" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:9" ht="15">
       <c r="A107" s="20" t="b">
         <v>0</v>
       </c>
@@ -8862,7 +8840,7 @@
       <c r="H107" s="20"/>
       <c r="I107" s="20"/>
     </row>
-    <row r="108" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:9" ht="15">
       <c r="A108" s="20"/>
       <c r="B108" s="20" t="s">
         <v>25</v>
@@ -8887,7 +8865,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="109" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:9" ht="15">
       <c r="A109" s="20"/>
       <c r="B109" s="20" t="s">
         <v>25</v>
@@ -8910,7 +8888,7 @@
       </c>
       <c r="I109" s="20"/>
     </row>
-    <row r="110" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:9" ht="15">
       <c r="A110" s="20"/>
       <c r="B110" s="20" t="s">
         <v>25</v>
@@ -8933,7 +8911,7 @@
       </c>
       <c r="I110" s="20"/>
     </row>
-    <row r="111" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:9" ht="15">
       <c r="A111" s="20"/>
       <c r="B111" s="20" t="s">
         <v>25</v>
@@ -8956,7 +8934,7 @@
       </c>
       <c r="I111" s="20"/>
     </row>
-    <row r="112" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:9" ht="15">
       <c r="A112" s="20"/>
       <c r="B112" s="20" t="s">
         <v>25</v>
@@ -8979,7 +8957,7 @@
       </c>
       <c r="I112" s="20"/>
     </row>
-    <row r="113" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:9" ht="15">
       <c r="A113" s="20"/>
       <c r="B113" s="20" t="s">
         <v>25</v>
@@ -9002,7 +8980,7 @@
       </c>
       <c r="I113" s="20"/>
     </row>
-    <row r="114" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:9" ht="15">
       <c r="A114" s="20"/>
       <c r="B114" s="20" t="s">
         <v>25</v>
@@ -9025,7 +9003,7 @@
       </c>
       <c r="I114" s="20"/>
     </row>
-    <row r="115" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:9" ht="15">
       <c r="A115" s="20" t="b">
         <v>0</v>
       </c>
@@ -9044,7 +9022,7 @@
       <c r="H115" s="20"/>
       <c r="I115" s="20"/>
     </row>
-    <row r="116" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:9" ht="15">
       <c r="A116" s="20"/>
       <c r="B116" s="20" t="s">
         <v>25</v>
@@ -9067,7 +9045,7 @@
       </c>
       <c r="I116" s="20"/>
     </row>
-    <row r="117" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:9" ht="15">
       <c r="A117" s="20"/>
       <c r="B117" s="20" t="s">
         <v>25</v>
@@ -9090,7 +9068,7 @@
       </c>
       <c r="I117" s="20"/>
     </row>
-    <row r="118" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:9" ht="15">
       <c r="A118" s="20"/>
       <c r="B118" s="20" t="s">
         <v>25</v>
@@ -9113,7 +9091,7 @@
       </c>
       <c r="I118" s="20"/>
     </row>
-    <row r="119" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:9" ht="15">
       <c r="A119" s="20" t="b">
         <v>0</v>
       </c>
@@ -9132,7 +9110,7 @@
       <c r="H119" s="20"/>
       <c r="I119" s="20"/>
     </row>
-    <row r="120" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:9" ht="15">
       <c r="A120" s="20"/>
       <c r="B120" s="20" t="s">
         <v>25</v>
@@ -9155,7 +9133,7 @@
       </c>
       <c r="I120" s="20"/>
     </row>
-    <row r="121" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:9" ht="15">
       <c r="A121" s="20"/>
       <c r="B121" s="20" t="s">
         <v>25</v>
@@ -9178,7 +9156,7 @@
       </c>
       <c r="I121" s="20"/>
     </row>
-    <row r="122" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:9" ht="15">
       <c r="A122" s="20"/>
       <c r="B122" s="20" t="s">
         <v>25</v>
@@ -9201,7 +9179,7 @@
       </c>
       <c r="I122" s="20"/>
     </row>
-    <row r="123" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:9" ht="15">
       <c r="A123" s="20"/>
       <c r="B123" s="20" t="s">
         <v>25</v>
@@ -9224,7 +9202,7 @@
       </c>
       <c r="I123" s="20"/>
     </row>
-    <row r="124" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:9" ht="15">
       <c r="A124" s="20"/>
       <c r="B124" s="20" t="s">
         <v>25</v>
@@ -9247,7 +9225,7 @@
       </c>
       <c r="I124" s="20"/>
     </row>
-    <row r="125" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:9" ht="15">
       <c r="A125" s="20"/>
       <c r="B125" s="20" t="s">
         <v>25</v>
@@ -9270,7 +9248,7 @@
       </c>
       <c r="I125" s="20"/>
     </row>
-    <row r="126" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:9" ht="15">
       <c r="A126" s="20" t="b">
         <v>0</v>
       </c>
@@ -9289,7 +9267,7 @@
       <c r="H126" s="20"/>
       <c r="I126" s="20"/>
     </row>
-    <row r="127" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:9" ht="15">
       <c r="A127" s="20"/>
       <c r="B127" s="20" t="s">
         <v>25</v>
@@ -9314,7 +9292,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="128" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:9" ht="15">
       <c r="A128" s="20"/>
       <c r="B128" s="20" t="s">
         <v>25</v>
@@ -9337,7 +9315,7 @@
       </c>
       <c r="I128" s="20"/>
     </row>
-    <row r="129" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:9" ht="15">
       <c r="A129" s="20"/>
       <c r="B129" s="20" t="s">
         <v>25</v>
@@ -9360,7 +9338,7 @@
       </c>
       <c r="I129" s="20"/>
     </row>
-    <row r="130" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:9" ht="15">
       <c r="A130" s="20"/>
       <c r="B130" s="20" t="s">
         <v>25</v>
@@ -9383,7 +9361,7 @@
       </c>
       <c r="I130" s="20"/>
     </row>
-    <row r="131" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:9" ht="15">
       <c r="A131" s="20"/>
       <c r="B131" s="20" t="s">
         <v>25</v>
@@ -9406,7 +9384,7 @@
       </c>
       <c r="I131" s="20"/>
     </row>
-    <row r="132" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:9" ht="15">
       <c r="A132" s="20"/>
       <c r="B132" s="20" t="s">
         <v>25</v>
@@ -9429,7 +9407,7 @@
       </c>
       <c r="I132" s="20"/>
     </row>
-    <row r="133" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:9" ht="15">
       <c r="A133" s="20"/>
       <c r="B133" s="20" t="s">
         <v>25</v>
@@ -9452,7 +9430,7 @@
       </c>
       <c r="I133" s="20"/>
     </row>
-    <row r="134" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:9" ht="15">
       <c r="A134" s="20"/>
       <c r="B134" s="20" t="s">
         <v>25</v>
@@ -9475,7 +9453,7 @@
       </c>
       <c r="I134" s="20"/>
     </row>
-    <row r="135" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:9" ht="15">
       <c r="A135" s="20"/>
       <c r="B135" s="20" t="s">
         <v>25</v>
@@ -9498,7 +9476,7 @@
       </c>
       <c r="I135" s="20"/>
     </row>
-    <row r="136" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:9" ht="15">
       <c r="A136" s="20" t="b">
         <v>0</v>
       </c>
@@ -9517,7 +9495,7 @@
       <c r="H136" s="20"/>
       <c r="I136" s="20"/>
     </row>
-    <row r="137" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:9" ht="15">
       <c r="A137" s="20"/>
       <c r="B137" s="20" t="s">
         <v>25</v>
@@ -9542,7 +9520,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="138" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:9" ht="15">
       <c r="A138" s="20"/>
       <c r="B138" s="20" t="s">
         <v>25</v>
@@ -9563,7 +9541,7 @@
       <c r="H138" s="20"/>
       <c r="I138" s="20"/>
     </row>
-    <row r="139" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:9" ht="15">
       <c r="A139" s="20"/>
       <c r="B139" s="20" t="s">
         <v>25</v>
@@ -9586,7 +9564,7 @@
       </c>
       <c r="I139" s="20"/>
     </row>
-    <row r="140" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:9" ht="15">
       <c r="A140" s="20"/>
       <c r="B140" s="20" t="s">
         <v>25</v>
@@ -9609,7 +9587,7 @@
       </c>
       <c r="I140" s="20"/>
     </row>
-    <row r="141" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:9" ht="15">
       <c r="A141" s="20"/>
       <c r="B141" s="20" t="s">
         <v>25</v>
@@ -9632,7 +9610,7 @@
       </c>
       <c r="I141" s="20"/>
     </row>
-    <row r="142" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:9" ht="15">
       <c r="A142" s="20"/>
       <c r="B142" s="20" t="s">
         <v>25</v>
@@ -9655,7 +9633,7 @@
       </c>
       <c r="I142" s="20"/>
     </row>
-    <row r="143" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:9" ht="15">
       <c r="A143" s="20"/>
       <c r="B143" s="20" t="s">
         <v>25</v>
@@ -9678,7 +9656,7 @@
       </c>
       <c r="I143" s="20"/>
     </row>
-    <row r="144" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:9" ht="15">
       <c r="A144" s="20"/>
       <c r="B144" s="20" t="s">
         <v>25</v>
@@ -9701,7 +9679,7 @@
       </c>
       <c r="I144" s="20"/>
     </row>
-    <row r="145" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:9" ht="15">
       <c r="A145" s="20"/>
       <c r="B145" s="20" t="s">
         <v>25</v>
@@ -9724,7 +9702,7 @@
       </c>
       <c r="I145" s="20"/>
     </row>
-    <row r="146" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:9" ht="15">
       <c r="A146" s="20"/>
       <c r="B146" s="20" t="s">
         <v>25</v>
@@ -9747,7 +9725,7 @@
       </c>
       <c r="I146" s="20"/>
     </row>
-    <row r="147" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:9" ht="15">
       <c r="A147" s="20"/>
       <c r="B147" s="20" t="s">
         <v>25</v>
@@ -9770,7 +9748,7 @@
       </c>
       <c r="I147" s="20"/>
     </row>
-    <row r="148" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:9" ht="15">
       <c r="A148" s="20"/>
       <c r="B148" s="20" t="s">
         <v>25</v>
@@ -9793,7 +9771,7 @@
       </c>
       <c r="I148" s="20"/>
     </row>
-    <row r="149" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:9" ht="15">
       <c r="A149" s="20"/>
       <c r="B149" s="20" t="s">
         <v>25</v>
@@ -9816,7 +9794,7 @@
       </c>
       <c r="I149" s="20"/>
     </row>
-    <row r="150" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:9" ht="15">
       <c r="A150" s="20"/>
       <c r="B150" s="20" t="s">
         <v>25</v>
@@ -9839,7 +9817,7 @@
       </c>
       <c r="I150" s="20"/>
     </row>
-    <row r="151" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:9" ht="15">
       <c r="A151" s="20" t="b">
         <v>0</v>
       </c>
@@ -9858,7 +9836,7 @@
       <c r="H151" s="20"/>
       <c r="I151" s="20"/>
     </row>
-    <row r="152" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:9" ht="15">
       <c r="A152" s="20"/>
       <c r="B152" s="20" t="s">
         <v>25</v>
@@ -9881,7 +9859,7 @@
       </c>
       <c r="I152" s="20"/>
     </row>
-    <row r="153" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:9" ht="15">
       <c r="A153" s="20" t="b">
         <v>0</v>
       </c>
@@ -9900,7 +9878,7 @@
       <c r="H153" s="20"/>
       <c r="I153" s="20"/>
     </row>
-    <row r="154" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:9" ht="15">
       <c r="A154" s="20"/>
       <c r="B154" s="20" t="s">
         <v>25</v>
@@ -9923,7 +9901,7 @@
       </c>
       <c r="I154" s="20"/>
     </row>
-    <row r="155" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:9" ht="15">
       <c r="A155" s="20"/>
       <c r="B155" s="20" t="s">
         <v>25</v>
@@ -9946,7 +9924,7 @@
       </c>
       <c r="I155" s="20"/>
     </row>
-    <row r="156" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:9" ht="15">
       <c r="A156" s="20" t="b">
         <v>0</v>
       </c>
@@ -9965,7 +9943,7 @@
       <c r="H156" s="20"/>
       <c r="I156" s="20"/>
     </row>
-    <row r="157" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:9" ht="15">
       <c r="A157" s="20"/>
       <c r="B157" s="20" t="s">
         <v>25</v>
@@ -9990,7 +9968,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="158" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:9" ht="15">
       <c r="A158" s="20"/>
       <c r="B158" s="20" t="s">
         <v>25</v>
@@ -10013,7 +9991,7 @@
       </c>
       <c r="I158" s="20"/>
     </row>
-    <row r="159" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:9" ht="15">
       <c r="A159" s="20"/>
       <c r="B159" s="20" t="s">
         <v>25</v>
@@ -10036,7 +10014,7 @@
       </c>
       <c r="I159" s="20"/>
     </row>
-    <row r="160" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:9" ht="15">
       <c r="A160" s="20"/>
       <c r="B160" s="20" t="s">
         <v>25</v>
@@ -10059,7 +10037,7 @@
       </c>
       <c r="I160" s="20"/>
     </row>
-    <row r="161" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:9" ht="15">
       <c r="A161" s="20"/>
       <c r="B161" s="20" t="s">
         <v>25</v>
@@ -10082,7 +10060,7 @@
       </c>
       <c r="I161" s="20"/>
     </row>
-    <row r="162" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:9" ht="15">
       <c r="A162" s="20"/>
       <c r="B162" s="20" t="s">
         <v>25</v>
@@ -10105,7 +10083,7 @@
       </c>
       <c r="I162" s="20"/>
     </row>
-    <row r="163" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:9" ht="15">
       <c r="A163" s="20"/>
       <c r="B163" s="20" t="s">
         <v>25</v>
@@ -10128,7 +10106,7 @@
       </c>
       <c r="I163" s="20"/>
     </row>
-    <row r="164" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:9" ht="15">
       <c r="A164" s="20"/>
       <c r="B164" s="20" t="s">
         <v>25</v>
@@ -10151,7 +10129,7 @@
       </c>
       <c r="I164" s="20"/>
     </row>
-    <row r="165" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:9" ht="15">
       <c r="A165" s="20"/>
       <c r="B165" s="20" t="s">
         <v>25</v>
@@ -10174,7 +10152,7 @@
       </c>
       <c r="I165" s="20"/>
     </row>
-    <row r="166" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:9" ht="15">
       <c r="A166" s="20"/>
       <c r="B166" s="20" t="s">
         <v>25</v>
@@ -10197,7 +10175,7 @@
       </c>
       <c r="I166" s="20"/>
     </row>
-    <row r="167" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:9" ht="15">
       <c r="A167" s="20" t="b">
         <v>0</v>
       </c>
@@ -10216,7 +10194,7 @@
       <c r="H167" s="20"/>
       <c r="I167" s="20"/>
     </row>
-    <row r="168" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:9" ht="15">
       <c r="A168" s="20"/>
       <c r="B168" s="20" t="s">
         <v>25</v>
@@ -10241,7 +10219,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="169" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:9" ht="15">
       <c r="A169" s="20"/>
       <c r="B169" s="20" t="s">
         <v>25</v>
@@ -10264,7 +10242,7 @@
       </c>
       <c r="I169" s="20"/>
     </row>
-    <row r="170" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:9" ht="15">
       <c r="A170" s="20"/>
       <c r="B170" s="20" t="s">
         <v>25</v>
@@ -10287,7 +10265,7 @@
       </c>
       <c r="I170" s="20"/>
     </row>
-    <row r="171" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:9" ht="15">
       <c r="A171" s="20"/>
       <c r="B171" s="20" t="s">
         <v>25</v>
@@ -10310,7 +10288,7 @@
       </c>
       <c r="I171" s="20"/>
     </row>
-    <row r="172" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:9" ht="15">
       <c r="A172" s="20"/>
       <c r="B172" s="20" t="s">
         <v>25</v>
@@ -10333,7 +10311,7 @@
       </c>
       <c r="I172" s="20"/>
     </row>
-    <row r="173" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:9" ht="15">
       <c r="A173" s="20"/>
       <c r="B173" s="20" t="s">
         <v>25</v>
@@ -10356,7 +10334,7 @@
       </c>
       <c r="I173" s="20"/>
     </row>
-    <row r="174" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:9" ht="15">
       <c r="A174" s="20"/>
       <c r="B174" s="20" t="s">
         <v>25</v>
@@ -10379,7 +10357,7 @@
       </c>
       <c r="I174" s="20"/>
     </row>
-    <row r="175" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:9" ht="15">
       <c r="A175" s="20"/>
       <c r="B175" s="20" t="s">
         <v>25</v>
@@ -10402,7 +10380,7 @@
       </c>
       <c r="I175" s="20"/>
     </row>
-    <row r="176" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:9" ht="15">
       <c r="A176" s="20"/>
       <c r="B176" s="20" t="s">
         <v>25</v>
@@ -10425,7 +10403,7 @@
       </c>
       <c r="I176" s="20"/>
     </row>
-    <row r="177" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:9" ht="15">
       <c r="A177" s="20"/>
       <c r="B177" s="20" t="s">
         <v>25</v>
@@ -10448,7 +10426,7 @@
       </c>
       <c r="I177" s="20"/>
     </row>
-    <row r="178" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:9" ht="15">
       <c r="A178" s="20" t="b">
         <v>0</v>
       </c>
@@ -10467,7 +10445,7 @@
       <c r="H178" s="20"/>
       <c r="I178" s="20"/>
     </row>
-    <row r="179" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:9" ht="15">
       <c r="A179" s="20"/>
       <c r="B179" s="20" t="s">
         <v>25</v>
@@ -10490,7 +10468,7 @@
       </c>
       <c r="I179" s="20"/>
     </row>
-    <row r="180" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:9" ht="15">
       <c r="A180" s="20"/>
       <c r="B180" s="20" t="s">
         <v>25</v>
@@ -10513,7 +10491,7 @@
       </c>
       <c r="I180" s="20"/>
     </row>
-    <row r="181" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:9" ht="15">
       <c r="A181" s="20"/>
       <c r="B181" s="20" t="s">
         <v>25</v>
@@ -10536,7 +10514,7 @@
       </c>
       <c r="I181" s="20"/>
     </row>
-    <row r="182" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:9" ht="15">
       <c r="A182" s="20"/>
       <c r="B182" s="20" t="s">
         <v>25</v>
@@ -10559,7 +10537,7 @@
       </c>
       <c r="I182" s="20"/>
     </row>
-    <row r="183" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:9" ht="15">
       <c r="A183" s="20" t="b">
         <v>0</v>
       </c>
@@ -10578,7 +10556,7 @@
       <c r="H183" s="20"/>
       <c r="I183" s="20"/>
     </row>
-    <row r="184" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:9" ht="15">
       <c r="A184" s="20"/>
       <c r="B184" s="20" t="s">
         <v>25</v>
@@ -10601,7 +10579,7 @@
       </c>
       <c r="I184" s="20"/>
     </row>
-    <row r="185" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:9" ht="15">
       <c r="A185" s="20"/>
       <c r="B185" s="20" t="s">
         <v>25</v>
@@ -10624,7 +10602,7 @@
       </c>
       <c r="I185" s="20"/>
     </row>
-    <row r="186" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:9" ht="15">
       <c r="A186" s="20"/>
       <c r="B186" s="20" t="s">
         <v>25</v>
@@ -10647,7 +10625,7 @@
       </c>
       <c r="I186" s="20"/>
     </row>
-    <row r="187" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:9" ht="15">
       <c r="A187" s="20"/>
       <c r="B187" s="20" t="s">
         <v>25</v>
@@ -10670,7 +10648,7 @@
       </c>
       <c r="I187" s="20"/>
     </row>
-    <row r="188" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:9" ht="15">
       <c r="A188" s="20" t="b">
         <v>0</v>
       </c>
@@ -10689,7 +10667,7 @@
       <c r="H188" s="20"/>
       <c r="I188" s="20"/>
     </row>
-    <row r="189" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:9" ht="15">
       <c r="A189" s="20"/>
       <c r="B189" s="20" t="s">
         <v>25</v>
@@ -10710,7 +10688,7 @@
       <c r="H189" s="20"/>
       <c r="I189" s="20"/>
     </row>
-    <row r="190" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:9" ht="15">
       <c r="A190" s="20"/>
       <c r="B190" s="20" t="s">
         <v>25</v>
@@ -10733,7 +10711,7 @@
       </c>
       <c r="I190" s="20"/>
     </row>
-    <row r="191" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:9" ht="15">
       <c r="A191" s="20" t="b">
         <v>0</v>
       </c>
@@ -10752,7 +10730,7 @@
       <c r="H191" s="20"/>
       <c r="I191" s="20"/>
     </row>
-    <row r="192" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:9" ht="15">
       <c r="A192" s="20"/>
       <c r="B192" s="20" t="s">
         <v>25</v>
@@ -10775,7 +10753,7 @@
       </c>
       <c r="I192" s="20"/>
     </row>
-    <row r="193" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:9" ht="15">
       <c r="A193" s="20"/>
       <c r="B193" s="20" t="s">
         <v>25</v>
@@ -10800,7 +10778,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="194" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:9" ht="15">
       <c r="A194" s="20"/>
       <c r="B194" s="20" t="s">
         <v>25</v>
@@ -10821,7 +10799,7 @@
       <c r="H194" s="20"/>
       <c r="I194" s="20"/>
     </row>
-    <row r="195" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:9" ht="15">
       <c r="A195" s="20"/>
       <c r="B195" s="20" t="s">
         <v>25</v>
@@ -10846,7 +10824,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="196" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:9" ht="15">
       <c r="A196" s="20"/>
       <c r="B196" s="20" t="s">
         <v>25</v>
@@ -10871,7 +10849,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="197" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:9" ht="15">
       <c r="A197" s="20" t="b">
         <v>0</v>
       </c>
@@ -10890,7 +10868,7 @@
       <c r="H197" s="20"/>
       <c r="I197" s="20"/>
     </row>
-    <row r="198" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:9" ht="15">
       <c r="A198" s="20"/>
       <c r="B198" s="20" t="s">
         <v>25</v>
@@ -10915,7 +10893,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="199" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:9" ht="15">
       <c r="A199" s="20"/>
       <c r="B199" s="20" t="s">
         <v>25</v>
@@ -10938,7 +10916,7 @@
       </c>
       <c r="I199" s="20"/>
     </row>
-    <row r="200" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:9" ht="15">
       <c r="A200" s="20"/>
       <c r="B200" s="20" t="s">
         <v>25</v>
@@ -10961,7 +10939,7 @@
       </c>
       <c r="I200" s="20"/>
     </row>
-    <row r="201" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:9" ht="15">
       <c r="A201" s="20"/>
       <c r="B201" s="20" t="s">
         <v>25</v>
@@ -10984,7 +10962,7 @@
       </c>
       <c r="I201" s="20"/>
     </row>
-    <row r="202" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:9" ht="15">
       <c r="A202" s="20"/>
       <c r="B202" s="20" t="s">
         <v>25</v>
@@ -11007,7 +10985,7 @@
       </c>
       <c r="I202" s="20"/>
     </row>
-    <row r="203" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:9" ht="15">
       <c r="A203" s="20"/>
       <c r="B203" s="20" t="s">
         <v>25</v>
@@ -11030,7 +11008,7 @@
       </c>
       <c r="I203" s="20"/>
     </row>
-    <row r="204" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:9" ht="15">
       <c r="A204" s="20"/>
       <c r="B204" s="20" t="s">
         <v>25</v>
@@ -11053,7 +11031,7 @@
       </c>
       <c r="I204" s="20"/>
     </row>
-    <row r="205" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:9" ht="15">
       <c r="A205" s="20"/>
       <c r="B205" s="20" t="s">
         <v>25</v>
@@ -11076,7 +11054,7 @@
       </c>
       <c r="I205" s="20"/>
     </row>
-    <row r="206" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:9" ht="15">
       <c r="A206" s="20"/>
       <c r="B206" s="20" t="s">
         <v>25</v>
@@ -11099,7 +11077,7 @@
       </c>
       <c r="I206" s="20"/>
     </row>
-    <row r="207" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:9" ht="15">
       <c r="A207" s="20" t="b">
         <v>0</v>
       </c>
@@ -11118,7 +11096,7 @@
       <c r="H207" s="20"/>
       <c r="I207" s="20"/>
     </row>
-    <row r="208" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:9" ht="15">
       <c r="A208" s="20"/>
       <c r="B208" s="20" t="s">
         <v>25</v>
@@ -11143,7 +11121,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="209" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:9" ht="15">
       <c r="A209" s="20"/>
       <c r="B209" s="20" t="s">
         <v>25</v>
@@ -11166,7 +11144,7 @@
       </c>
       <c r="I209" s="20"/>
     </row>
-    <row r="210" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:9" ht="15">
       <c r="A210" s="20"/>
       <c r="B210" s="20" t="s">
         <v>25</v>
@@ -11189,7 +11167,7 @@
       </c>
       <c r="I210" s="20"/>
     </row>
-    <row r="211" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:9" ht="15">
       <c r="A211" s="20"/>
       <c r="B211" s="20" t="s">
         <v>25</v>
@@ -11212,7 +11190,7 @@
       </c>
       <c r="I211" s="20"/>
     </row>
-    <row r="212" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:9" ht="15">
       <c r="A212" s="20"/>
       <c r="B212" s="20" t="s">
         <v>25</v>
@@ -11235,7 +11213,7 @@
       </c>
       <c r="I212" s="20"/>
     </row>
-    <row r="213" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:9" ht="15">
       <c r="A213" s="20"/>
       <c r="B213" s="20" t="s">
         <v>25</v>
@@ -11258,7 +11236,7 @@
       </c>
       <c r="I213" s="20"/>
     </row>
-    <row r="214" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:9" ht="15">
       <c r="A214" s="20"/>
       <c r="B214" s="20" t="s">
         <v>25</v>
@@ -11281,7 +11259,7 @@
       </c>
       <c r="I214" s="20"/>
     </row>
-    <row r="215" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:9" ht="15">
       <c r="A215" s="20"/>
       <c r="B215" s="20" t="s">
         <v>25</v>
@@ -11304,7 +11282,7 @@
       </c>
       <c r="I215" s="20"/>
     </row>
-    <row r="216" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:9" ht="15">
       <c r="A216" s="20"/>
       <c r="B216" s="20" t="s">
         <v>25</v>
@@ -11327,7 +11305,7 @@
       </c>
       <c r="I216" s="20"/>
     </row>
-    <row r="217" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:9" ht="15">
       <c r="A217" s="20" t="b">
         <v>0</v>
       </c>
@@ -11346,7 +11324,7 @@
       <c r="H217" s="20"/>
       <c r="I217" s="20"/>
     </row>
-    <row r="218" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:9" ht="15">
       <c r="A218" s="20"/>
       <c r="B218" s="20" t="s">
         <v>25</v>
@@ -11367,7 +11345,7 @@
       <c r="H218" s="20"/>
       <c r="I218" s="20"/>
     </row>
-    <row r="219" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:9" ht="15">
       <c r="A219" s="20"/>
       <c r="B219" s="20" t="s">
         <v>25</v>
@@ -11390,7 +11368,7 @@
       </c>
       <c r="I219" s="20"/>
     </row>
-    <row r="220" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:9" ht="15">
       <c r="A220" s="20"/>
       <c r="B220" s="20" t="s">
         <v>25</v>
@@ -11413,7 +11391,7 @@
       </c>
       <c r="I220" s="20"/>
     </row>
-    <row r="221" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:9" ht="15">
       <c r="A221" s="20"/>
       <c r="B221" s="20" t="s">
         <v>25</v>
@@ -11436,7 +11414,7 @@
       </c>
       <c r="I221" s="20"/>
     </row>
-    <row r="222" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:9" ht="15">
       <c r="A222" s="20"/>
       <c r="B222" s="20" t="s">
         <v>25</v>
@@ -11459,7 +11437,7 @@
       </c>
       <c r="I222" s="20"/>
     </row>
-    <row r="223" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:9" ht="15">
       <c r="A223" s="20"/>
       <c r="B223" s="20" t="s">
         <v>25</v>
@@ -11482,7 +11460,7 @@
       </c>
       <c r="I223" s="20"/>
     </row>
-    <row r="224" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:9" ht="15">
       <c r="A224" s="20"/>
       <c r="B224" s="20" t="s">
         <v>25</v>
@@ -11505,7 +11483,7 @@
       </c>
       <c r="I224" s="20"/>
     </row>
-    <row r="225" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:9" ht="15">
       <c r="A225" s="20"/>
       <c r="B225" s="20" t="s">
         <v>25</v>
@@ -11528,7 +11506,7 @@
       </c>
       <c r="I225" s="20"/>
     </row>
-    <row r="226" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:9" ht="15">
       <c r="A226" s="20"/>
       <c r="B226" s="20" t="s">
         <v>25</v>
@@ -11551,7 +11529,7 @@
       </c>
       <c r="I226" s="20"/>
     </row>
-    <row r="227" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:9" ht="15">
       <c r="A227" s="20"/>
       <c r="B227" s="20" t="s">
         <v>25</v>
@@ -11574,7 +11552,7 @@
       </c>
       <c r="I227" s="20"/>
     </row>
-    <row r="228" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:9" ht="15">
       <c r="A228" s="20"/>
       <c r="B228" s="20" t="s">
         <v>25</v>
@@ -11597,7 +11575,7 @@
       </c>
       <c r="I228" s="20"/>
     </row>
-    <row r="229" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:9" ht="15">
       <c r="A229" s="20"/>
       <c r="B229" s="20" t="s">
         <v>25</v>
@@ -11620,7 +11598,7 @@
       </c>
       <c r="I229" s="20"/>
     </row>
-    <row r="230" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:9" ht="15">
       <c r="A230" s="20"/>
       <c r="B230" s="20" t="s">
         <v>25</v>
@@ -11643,7 +11621,7 @@
       </c>
       <c r="I230" s="20"/>
     </row>
-    <row r="231" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:9" ht="15">
       <c r="A231" s="20"/>
       <c r="B231" s="20" t="s">
         <v>25</v>
@@ -11666,7 +11644,7 @@
       </c>
       <c r="I231" s="20"/>
     </row>
-    <row r="232" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:9" ht="15">
       <c r="A232" s="20"/>
       <c r="B232" s="20" t="s">
         <v>25</v>
@@ -11689,7 +11667,7 @@
       </c>
       <c r="I232" s="20"/>
     </row>
-    <row r="233" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:9" ht="15">
       <c r="A233" s="20"/>
       <c r="B233" s="20" t="s">
         <v>25</v>
@@ -11712,7 +11690,7 @@
       </c>
       <c r="I233" s="20"/>
     </row>
-    <row r="234" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:9" ht="15">
       <c r="A234" s="20" t="b">
         <v>0</v>
       </c>
@@ -11731,7 +11709,7 @@
       <c r="H234" s="20"/>
       <c r="I234" s="20"/>
     </row>
-    <row r="235" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:9" ht="15">
       <c r="A235" s="20"/>
       <c r="B235" s="20" t="s">
         <v>25</v>
@@ -11752,7 +11730,7 @@
       <c r="H235" s="20"/>
       <c r="I235" s="20"/>
     </row>
-    <row r="236" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:9" ht="15">
       <c r="A236" s="20"/>
       <c r="B236" s="20" t="s">
         <v>25</v>
@@ -11775,7 +11753,7 @@
       </c>
       <c r="I236" s="20"/>
     </row>
-    <row r="237" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:9" ht="15">
       <c r="A237" s="20"/>
       <c r="B237" s="20" t="s">
         <v>25</v>
@@ -11798,7 +11776,7 @@
       </c>
       <c r="I237" s="20"/>
     </row>
-    <row r="238" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:9" ht="15">
       <c r="A238" s="20"/>
       <c r="B238" s="20" t="s">
         <v>25</v>
@@ -11821,7 +11799,7 @@
       </c>
       <c r="I238" s="20"/>
     </row>
-    <row r="239" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:9" ht="15">
       <c r="A239" s="20"/>
       <c r="B239" s="20" t="s">
         <v>25</v>
@@ -11844,7 +11822,7 @@
       </c>
       <c r="I239" s="20"/>
     </row>
-    <row r="240" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:9" ht="15">
       <c r="A240" s="20"/>
       <c r="B240" s="20" t="s">
         <v>25</v>
@@ -11867,7 +11845,7 @@
       </c>
       <c r="I240" s="20"/>
     </row>
-    <row r="241" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:9" ht="15">
       <c r="A241" s="20"/>
       <c r="B241" s="20" t="s">
         <v>25</v>
@@ -11890,7 +11868,7 @@
       </c>
       <c r="I241" s="20"/>
     </row>
-    <row r="242" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:9" ht="15">
       <c r="A242" s="20"/>
       <c r="B242" s="20" t="s">
         <v>25</v>
@@ -11913,7 +11891,7 @@
       </c>
       <c r="I242" s="20"/>
     </row>
-    <row r="243" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:9" ht="15">
       <c r="A243" s="20"/>
       <c r="B243" s="20" t="s">
         <v>25</v>
@@ -11936,7 +11914,7 @@
       </c>
       <c r="I243" s="20"/>
     </row>
-    <row r="244" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:9" ht="15">
       <c r="A244" s="20"/>
       <c r="B244" s="20" t="s">
         <v>25</v>
@@ -11959,7 +11937,7 @@
       </c>
       <c r="I244" s="20"/>
     </row>
-    <row r="245" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:9" ht="15">
       <c r="A245" s="20"/>
       <c r="B245" s="20" t="s">
         <v>25</v>
@@ -11982,7 +11960,7 @@
       </c>
       <c r="I245" s="20"/>
     </row>
-    <row r="246" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:9" ht="15">
       <c r="A246" s="20"/>
       <c r="B246" s="20" t="s">
         <v>25</v>
@@ -12005,7 +11983,7 @@
       </c>
       <c r="I246" s="20"/>
     </row>
-    <row r="247" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:9" ht="15">
       <c r="A247" s="20"/>
       <c r="B247" s="20" t="s">
         <v>25</v>
@@ -12028,7 +12006,7 @@
       </c>
       <c r="I247" s="20"/>
     </row>
-    <row r="248" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:9" ht="15">
       <c r="A248" s="20"/>
       <c r="B248" s="20" t="s">
         <v>25</v>
@@ -12051,7 +12029,7 @@
       </c>
       <c r="I248" s="20"/>
     </row>
-    <row r="249" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:9" ht="15">
       <c r="A249" s="20"/>
       <c r="B249" s="20" t="s">
         <v>25</v>
@@ -12074,7 +12052,7 @@
       </c>
       <c r="I249" s="20"/>
     </row>
-    <row r="250" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:9" ht="15">
       <c r="A250" s="20"/>
       <c r="B250" s="20" t="s">
         <v>25</v>
@@ -12097,7 +12075,7 @@
       </c>
       <c r="I250" s="20"/>
     </row>
-    <row r="251" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:9" ht="15">
       <c r="A251" s="20" t="b">
         <v>0</v>
       </c>
@@ -12116,7 +12094,7 @@
       <c r="H251" s="20"/>
       <c r="I251" s="20"/>
     </row>
-    <row r="252" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:9" ht="15">
       <c r="A252" s="20"/>
       <c r="B252" s="20" t="s">
         <v>25</v>
@@ -12141,7 +12119,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="253" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:9" ht="15">
       <c r="A253" s="20"/>
       <c r="B253" s="20" t="s">
         <v>25</v>
@@ -12164,7 +12142,7 @@
       </c>
       <c r="I253" s="20"/>
     </row>
-    <row r="254" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:9" ht="15">
       <c r="A254" s="20"/>
       <c r="B254" s="20" t="s">
         <v>25</v>
@@ -12187,7 +12165,7 @@
       </c>
       <c r="I254" s="20"/>
     </row>
-    <row r="255" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:9" ht="15">
       <c r="A255" s="20"/>
       <c r="B255" s="20" t="s">
         <v>25</v>
@@ -12210,7 +12188,7 @@
       </c>
       <c r="I255" s="20"/>
     </row>
-    <row r="256" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:9" ht="15">
       <c r="A256" s="20"/>
       <c r="B256" s="20" t="s">
         <v>25</v>
@@ -12233,7 +12211,7 @@
       </c>
       <c r="I256" s="20"/>
     </row>
-    <row r="257" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:9" ht="15">
       <c r="A257" s="20" t="b">
         <v>0</v>
       </c>
@@ -12252,7 +12230,7 @@
       <c r="H257" s="20"/>
       <c r="I257" s="20"/>
     </row>
-    <row r="258" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:9" ht="15">
       <c r="A258" s="20"/>
       <c r="B258" s="20" t="s">
         <v>25</v>
@@ -12277,7 +12255,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="259" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:9" ht="15">
       <c r="A259" s="20"/>
       <c r="B259" s="20" t="s">
         <v>25</v>
@@ -12300,7 +12278,7 @@
       </c>
       <c r="I259" s="20"/>
     </row>
-    <row r="260" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:9" ht="15">
       <c r="A260" s="20" t="b">
         <v>0</v>
       </c>
@@ -12319,7 +12297,7 @@
       <c r="H260" s="20"/>
       <c r="I260" s="20"/>
     </row>
-    <row r="261" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:9" ht="15">
       <c r="A261" s="20" t="b">
         <v>0</v>
       </c>
@@ -12338,7 +12316,7 @@
       <c r="H261" s="20"/>
       <c r="I261" s="20"/>
     </row>
-    <row r="262" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:9" ht="15">
       <c r="A262" s="20" t="b">
         <v>0</v>
       </c>
@@ -12357,7 +12335,7 @@
       <c r="H262" s="20"/>
       <c r="I262" s="20"/>
     </row>
-    <row r="263" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:9" ht="15">
       <c r="A263" s="20"/>
       <c r="B263" s="20" t="s">
         <v>25</v>
@@ -12378,7 +12356,7 @@
       <c r="H263" s="20"/>
       <c r="I263" s="20"/>
     </row>
-    <row r="264" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:9" ht="15">
       <c r="A264" s="20"/>
       <c r="B264" s="20" t="s">
         <v>25</v>
@@ -12401,7 +12379,7 @@
       </c>
       <c r="I264" s="20"/>
     </row>
-    <row r="265" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:9" ht="15">
       <c r="A265" s="20"/>
       <c r="B265" s="20" t="s">
         <v>25</v>
@@ -12424,7 +12402,7 @@
       </c>
       <c r="I265" s="20"/>
     </row>
-    <row r="266" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:9" ht="15">
       <c r="A266" s="20"/>
       <c r="B266" s="20" t="s">
         <v>25</v>
@@ -12447,7 +12425,7 @@
       </c>
       <c r="I266" s="20"/>
     </row>
-    <row r="267" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:9" ht="15">
       <c r="A267" s="20"/>
       <c r="B267" s="20" t="s">
         <v>25</v>
@@ -12470,7 +12448,7 @@
       </c>
       <c r="I267" s="20"/>
     </row>
-    <row r="268" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:9" ht="15">
       <c r="A268" s="20"/>
       <c r="B268" s="20" t="s">
         <v>25</v>
@@ -12493,7 +12471,7 @@
       </c>
       <c r="I268" s="20"/>
     </row>
-    <row r="269" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:9" ht="15">
       <c r="A269" s="20"/>
       <c r="B269" s="20" t="s">
         <v>25</v>
@@ -12516,7 +12494,7 @@
       </c>
       <c r="I269" s="20"/>
     </row>
-    <row r="270" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:9" ht="15">
       <c r="A270" s="20"/>
       <c r="B270" s="20" t="s">
         <v>25</v>
@@ -12539,7 +12517,7 @@
       </c>
       <c r="I270" s="20"/>
     </row>
-    <row r="271" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:9" ht="15">
       <c r="A271" s="20"/>
       <c r="B271" s="20" t="s">
         <v>25</v>
@@ -12562,7 +12540,7 @@
       </c>
       <c r="I271" s="20"/>
     </row>
-    <row r="272" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:9" ht="15">
       <c r="A272" s="20"/>
       <c r="B272" s="20" t="s">
         <v>25</v>
@@ -12585,7 +12563,7 @@
       </c>
       <c r="I272" s="20"/>
     </row>
-    <row r="273" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:9" ht="15">
       <c r="A273" s="20"/>
       <c r="B273" s="20" t="s">
         <v>25</v>
@@ -12608,7 +12586,7 @@
       </c>
       <c r="I273" s="20"/>
     </row>
-    <row r="274" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:9" ht="15">
       <c r="A274" s="20" t="b">
         <v>0</v>
       </c>
@@ -12627,7 +12605,7 @@
       <c r="H274" s="20"/>
       <c r="I274" s="20"/>
     </row>
-    <row r="275" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:9" ht="15">
       <c r="A275" s="20"/>
       <c r="B275" s="20" t="s">
         <v>25</v>
@@ -12650,7 +12628,7 @@
       </c>
       <c r="I275" s="20"/>
     </row>
-    <row r="276" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:9" ht="15">
       <c r="A276" s="20" t="b">
         <v>0</v>
       </c>
@@ -12669,7 +12647,7 @@
       <c r="H276" s="20"/>
       <c r="I276" s="20"/>
     </row>
-    <row r="277" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:9" ht="15">
       <c r="A277" s="20"/>
       <c r="B277" s="20" t="s">
         <v>25</v>
@@ -12694,7 +12672,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="278" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:9" ht="15">
       <c r="A278" s="20"/>
       <c r="B278" s="20" t="s">
         <v>25</v>
@@ -12717,7 +12695,7 @@
       </c>
       <c r="I278" s="20"/>
     </row>
-    <row r="279" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:9" ht="15">
       <c r="A279" s="20"/>
       <c r="B279" s="20" t="s">
         <v>25</v>
@@ -12740,7 +12718,7 @@
       </c>
       <c r="I279" s="20"/>
     </row>
-    <row r="280" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:9" ht="15">
       <c r="A280" s="20"/>
       <c r="B280" s="20" t="s">
         <v>25</v>
@@ -12763,7 +12741,7 @@
       </c>
       <c r="I280" s="20"/>
     </row>
-    <row r="281" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:9" ht="15">
       <c r="A281" s="20"/>
       <c r="B281" s="20" t="s">
         <v>25</v>
@@ -12786,7 +12764,7 @@
       </c>
       <c r="I281" s="20"/>
     </row>
-    <row r="282" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:9" ht="15">
       <c r="A282" s="20"/>
       <c r="B282" s="20" t="s">
         <v>25</v>
@@ -12809,7 +12787,7 @@
       </c>
       <c r="I282" s="20"/>
     </row>
-    <row r="283" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:9" ht="15">
       <c r="A283" s="20"/>
       <c r="B283" s="20" t="s">
         <v>25</v>
@@ -12832,7 +12810,7 @@
       </c>
       <c r="I283" s="20"/>
     </row>
-    <row r="284" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:9" ht="15">
       <c r="A284" s="20"/>
       <c r="B284" s="20" t="s">
         <v>25</v>
@@ -12855,7 +12833,7 @@
       </c>
       <c r="I284" s="20"/>
     </row>
-    <row r="285" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:9" ht="15">
       <c r="A285" s="20"/>
       <c r="B285" s="20" t="s">
         <v>25</v>
@@ -12878,7 +12856,7 @@
       </c>
       <c r="I285" s="20"/>
     </row>
-    <row r="286" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:9" ht="15">
       <c r="A286" s="20"/>
       <c r="B286" s="20" t="s">
         <v>25</v>
@@ -12901,7 +12879,7 @@
       </c>
       <c r="I286" s="20"/>
     </row>
-    <row r="287" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:9" ht="15">
       <c r="A287" s="20"/>
       <c r="B287" s="20" t="s">
         <v>25</v>
@@ -12924,7 +12902,7 @@
       </c>
       <c r="I287" s="20"/>
     </row>
-    <row r="288" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:9" ht="15">
       <c r="A288" s="20" t="b">
         <v>0</v>
       </c>
@@ -12943,7 +12921,7 @@
       <c r="H288" s="20"/>
       <c r="I288" s="20"/>
     </row>
-    <row r="289" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:9" ht="15">
       <c r="A289" s="20"/>
       <c r="B289" s="20" t="s">
         <v>25</v>
@@ -12966,7 +12944,7 @@
       </c>
       <c r="I289" s="20"/>
     </row>
-    <row r="290" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:9" ht="15">
       <c r="A290" s="20" t="b">
         <v>0</v>
       </c>
@@ -12985,7 +12963,7 @@
       <c r="H290" s="20"/>
       <c r="I290" s="20"/>
     </row>
-    <row r="291" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:9" ht="15">
       <c r="A291" s="20"/>
       <c r="B291" s="20" t="s">
         <v>25</v>
@@ -13006,7 +12984,7 @@
       <c r="H291" s="20"/>
       <c r="I291" s="20"/>
     </row>
-    <row r="292" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:9" ht="15">
       <c r="A292" s="20" t="b">
         <v>0</v>
       </c>
@@ -13025,7 +13003,7 @@
       <c r="H292" s="20"/>
       <c r="I292" s="20"/>
     </row>
-    <row r="293" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:9" ht="15">
       <c r="A293" s="20"/>
       <c r="B293" s="20" t="s">
         <v>25</v>
@@ -13046,7 +13024,7 @@
       <c r="H293" s="20"/>
       <c r="I293" s="20"/>
     </row>
-    <row r="294" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:9" ht="15">
       <c r="A294" s="20" t="b">
         <v>0</v>
       </c>
@@ -13065,7 +13043,7 @@
       <c r="H294" s="20"/>
       <c r="I294" s="20"/>
     </row>
-    <row r="295" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:9" ht="15">
       <c r="A295" s="20"/>
       <c r="B295" s="20" t="s">
         <v>25</v>
@@ -13086,7 +13064,7 @@
       <c r="H295" s="20"/>
       <c r="I295" s="20"/>
     </row>
-    <row r="296" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:9" ht="15">
       <c r="A296" s="20" t="b">
         <v>0</v>
       </c>
@@ -13105,7 +13083,7 @@
       <c r="H296" s="20"/>
       <c r="I296" s="20"/>
     </row>
-    <row r="297" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:9" ht="15">
       <c r="A297" s="20"/>
       <c r="B297" s="20" t="s">
         <v>25</v>
@@ -13128,7 +13106,7 @@
       </c>
       <c r="I297" s="20"/>
     </row>
-    <row r="298" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:9" ht="15">
       <c r="A298" s="20" t="b">
         <v>0</v>
       </c>
@@ -13147,7 +13125,7 @@
       <c r="H298" s="20"/>
       <c r="I298" s="20"/>
     </row>
-    <row r="299" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:9" ht="15">
       <c r="A299" s="20"/>
       <c r="B299" s="20" t="s">
         <v>25</v>
@@ -13172,7 +13150,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="300" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:9" ht="15">
       <c r="A300" s="20"/>
       <c r="B300" s="20" t="s">
         <v>25</v>
@@ -13195,7 +13173,7 @@
       </c>
       <c r="I300" s="20"/>
     </row>
-    <row r="301" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:9" ht="15">
       <c r="A301" s="20"/>
       <c r="B301" s="20" t="s">
         <v>25</v>
@@ -13218,7 +13196,7 @@
       </c>
       <c r="I301" s="20"/>
     </row>
-    <row r="302" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:9" ht="15">
       <c r="A302" s="20"/>
       <c r="B302" s="20" t="s">
         <v>25</v>
@@ -13241,7 +13219,7 @@
       </c>
       <c r="I302" s="20"/>
     </row>
-    <row r="303" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:9" ht="15">
       <c r="A303" s="20"/>
       <c r="B303" s="20" t="s">
         <v>25</v>
@@ -13264,7 +13242,7 @@
       </c>
       <c r="I303" s="20"/>
     </row>
-    <row r="304" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:9" ht="15">
       <c r="A304" s="20"/>
       <c r="B304" s="20" t="s">
         <v>25</v>
@@ -13287,7 +13265,7 @@
       </c>
       <c r="I304" s="20"/>
     </row>
-    <row r="305" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:9" ht="15">
       <c r="A305" s="20"/>
       <c r="B305" s="20" t="s">
         <v>25</v>
@@ -13310,7 +13288,7 @@
       </c>
       <c r="I305" s="20"/>
     </row>
-    <row r="306" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:9" ht="15">
       <c r="A306" s="20"/>
       <c r="B306" s="20" t="s">
         <v>25</v>
@@ -13333,7 +13311,7 @@
       </c>
       <c r="I306" s="20"/>
     </row>
-    <row r="307" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:9" ht="15">
       <c r="A307" s="20"/>
       <c r="B307" s="20" t="s">
         <v>25</v>
@@ -13356,7 +13334,7 @@
       </c>
       <c r="I307" s="20"/>
     </row>
-    <row r="308" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:9" ht="15">
       <c r="A308" s="20" t="b">
         <v>0</v>
       </c>
@@ -13375,7 +13353,7 @@
       <c r="H308" s="20"/>
       <c r="I308" s="20"/>
     </row>
-    <row r="309" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:9" ht="15">
       <c r="A309" s="20"/>
       <c r="B309" s="20" t="s">
         <v>25</v>
@@ -13398,7 +13376,7 @@
       </c>
       <c r="I309" s="20"/>
     </row>
-    <row r="310" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:9" ht="15">
       <c r="A310" s="20"/>
       <c r="B310" s="20" t="s">
         <v>25</v>
@@ -13421,7 +13399,7 @@
       </c>
       <c r="I310" s="20"/>
     </row>
-    <row r="311" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:9" ht="15">
       <c r="A311" s="20"/>
       <c r="B311" s="20" t="s">
         <v>25</v>
@@ -13444,7 +13422,7 @@
       </c>
       <c r="I311" s="20"/>
     </row>
-    <row r="312" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:9" ht="15">
       <c r="A312" s="20"/>
       <c r="B312" s="20" t="s">
         <v>25</v>
@@ -13467,7 +13445,7 @@
       </c>
       <c r="I312" s="20"/>
     </row>
-    <row r="313" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:9" ht="15">
       <c r="A313" s="20" t="b">
         <v>0</v>
       </c>
@@ -13486,7 +13464,7 @@
       <c r="H313" s="20"/>
       <c r="I313" s="20"/>
     </row>
-    <row r="314" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:9" ht="15">
       <c r="A314" s="20"/>
       <c r="B314" s="20" t="s">
         <v>25</v>
@@ -13509,7 +13487,7 @@
       </c>
       <c r="I314" s="20"/>
     </row>
-    <row r="315" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:9" ht="15">
       <c r="A315" s="20"/>
       <c r="B315" s="20" t="s">
         <v>25</v>
@@ -13532,7 +13510,7 @@
       </c>
       <c r="I315" s="20"/>
     </row>
-    <row r="316" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:9" ht="15">
       <c r="A316" s="20"/>
       <c r="B316" s="20" t="s">
         <v>25</v>
@@ -13557,7 +13535,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="317" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:9" ht="15">
       <c r="A317" s="20" t="b">
         <v>0</v>
       </c>
@@ -13576,7 +13554,7 @@
       <c r="H317" s="20"/>
       <c r="I317" s="20"/>
     </row>
-    <row r="318" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:9" ht="15">
       <c r="A318" s="20"/>
       <c r="B318" s="20" t="s">
         <v>25</v>
@@ -13601,7 +13579,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="319" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:9" ht="15">
       <c r="A319" s="20"/>
       <c r="B319" s="20" t="s">
         <v>25</v>
@@ -13624,7 +13602,7 @@
       </c>
       <c r="I319" s="20"/>
     </row>
-    <row r="320" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="320" spans="1:9" ht="15">
       <c r="A320" s="20" t="b">
         <v>0</v>
       </c>
@@ -13643,7 +13621,7 @@
       <c r="H320" s="20"/>
       <c r="I320" s="20"/>
     </row>
-    <row r="321" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="321" spans="1:9" ht="15">
       <c r="A321" s="20"/>
       <c r="B321" s="20" t="s">
         <v>25</v>
@@ -13664,7 +13642,7 @@
       <c r="H321" s="20"/>
       <c r="I321" s="20"/>
     </row>
-    <row r="322" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="322" spans="1:9" ht="15">
       <c r="A322" s="20"/>
       <c r="B322" s="20" t="s">
         <v>25</v>
@@ -13685,7 +13663,7 @@
       <c r="H322" s="20"/>
       <c r="I322" s="20"/>
     </row>
-    <row r="323" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="323" spans="1:9" ht="15">
       <c r="A323" s="20"/>
       <c r="B323" s="20" t="s">
         <v>25</v>
@@ -13708,7 +13686,7 @@
       </c>
       <c r="I323" s="20"/>
     </row>
-    <row r="324" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:9" ht="15">
       <c r="A324" s="20" t="b">
         <v>0</v>
       </c>
@@ -13727,7 +13705,7 @@
       <c r="H324" s="20"/>
       <c r="I324" s="20"/>
     </row>
-    <row r="325" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="325" spans="1:9" ht="15">
       <c r="A325" s="20" t="b">
         <v>0</v>
       </c>
@@ -13746,7 +13724,7 @@
       <c r="H325" s="20"/>
       <c r="I325" s="20"/>
     </row>
-    <row r="326" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="326" spans="1:9" ht="15">
       <c r="A326" s="20"/>
       <c r="B326" s="20" t="s">
         <v>25</v>
@@ -13771,7 +13749,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="327" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="327" spans="1:9" ht="15">
       <c r="A327" s="20"/>
       <c r="B327" s="20" t="s">
         <v>25</v>
@@ -13814,13 +13792,13 @@
       <selection activeCell="A7" sqref="A7:A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>459</v>
       </c>
@@ -13831,7 +13809,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>449</v>
       </c>
@@ -13842,7 +13820,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>450</v>
       </c>
@@ -13853,7 +13831,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>457</v>
       </c>
@@ -13864,7 +13842,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>451</v>
       </c>
@@ -13875,17 +13853,17 @@
         <v>456</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
         <v>470</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
         <v>478</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
         <v>476</v>
       </c>

</xml_diff>